<commit_message>
add html wrapper. more doi handling
</commit_message>
<xml_diff>
--- a/contribs.xlsx
+++ b/contribs.xlsx
@@ -531,7 +531,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="8.86328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="22.1328125"/>
@@ -1648,7 +1648,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="8.86328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="21.86328125"/>
@@ -2696,7 +2696,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="24"/>
     <col customWidth="1" max="2" min="2" style="17" width="14.59765625"/>
@@ -5810,7 +5810,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="26.1328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="18.3984375"/>
@@ -10611,13 +10611,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="27.06640625"/>
     <col customWidth="1" max="2" min="2" style="17" width="41.19921875"/>
@@ -12418,10 +12418,6 @@
           <t>Crutchfield</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="76" s="17">
       <c r="A76" t="inlineStr">
@@ -12439,10 +12435,6 @@
           <t>Cho</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="77" s="17">
       <c r="A77" t="inlineStr">
@@ -12460,10 +12452,6 @@
           <t>Turecek</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="78" s="17">
       <c r="A78" t="inlineStr">
@@ -12481,10 +12469,6 @@
           <t>Botes</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="79" s="17">
       <c r="A79" t="inlineStr">
@@ -12502,10 +12486,6 @@
           <t>Berghoff</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="80" s="17">
       <c r="A80" t="inlineStr">
@@ -12523,10 +12503,6 @@
           <t>Donohoe</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="81" s="17">
       <c r="A81" t="inlineStr">
@@ -12544,10 +12520,6 @@
           <t>Seitz</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="82" s="17">
       <c r="A82" t="inlineStr">
@@ -12565,10 +12537,6 @@
           <t>Westphal</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="83" s="17">
       <c r="A83" t="inlineStr">
@@ -12586,10 +12554,6 @@
           <t>Dengscherz</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="84" s="17">
       <c r="A84" t="inlineStr">
@@ -12607,10 +12571,6 @@
           <t>Beckmann</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="85" s="17">
       <c r="A85" t="inlineStr">
@@ -12628,10 +12588,6 @@
           <t>Bryant</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="86" s="17">
       <c r="A86" t="inlineStr">
@@ -12649,10 +12605,6 @@
           <t>Sharp</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="87" s="17">
       <c r="A87" t="inlineStr">
@@ -12670,10 +12622,6 @@
           <t>Ilg</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="88" s="17">
       <c r="A88" t="inlineStr">
@@ -12691,10 +12639,6 @@
           <t>Kutzelmann</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="89" s="17">
       <c r="A89" t="inlineStr">
@@ -12712,10 +12656,6 @@
           <t>Massler</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="90" s="17">
       <c r="A90" t="inlineStr">
@@ -12733,10 +12673,6 @@
           <t>Peter</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="91" s="17">
       <c r="A91" t="inlineStr">
@@ -12754,10 +12690,6 @@
           <t>Theinert</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="92" s="17">
       <c r="A92" t="inlineStr">
@@ -12775,10 +12707,6 @@
           <t>Reinhardt</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="93" s="17">
       <c r="A93" t="inlineStr">
@@ -12796,10 +12724,6 @@
           <t>Capra</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.75" r="94" s="17">
       <c r="A94" t="inlineStr">
@@ -12817,32 +12741,368 @@
           <t>Paul</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr"/>
-    </row>
-    <row customHeight="1" ht="12.75" r="95" s="17"/>
-    <row customHeight="1" ht="12.75" r="96" s="17"/>
-    <row customHeight="1" ht="12.75" r="97" s="17"/>
-    <row customHeight="1" ht="12.75" r="98" s="17"/>
-    <row customHeight="1" ht="12.75" r="99" s="17"/>
-    <row customHeight="1" ht="12.75" r="100" s="17"/>
-    <row customHeight="1" ht="12.75" r="101" s="17"/>
-    <row customHeight="1" ht="12.75" r="102" s="17"/>
-    <row customHeight="1" ht="12.75" r="103" s="17"/>
-    <row customHeight="1" ht="12.75" r="104" s="17"/>
-    <row customHeight="1" ht="12.75" r="105" s="17"/>
-    <row customHeight="1" ht="12.75" r="106" s="17"/>
-    <row customHeight="1" ht="12.75" r="107" s="17"/>
-    <row customHeight="1" ht="12.75" r="108" s="17"/>
-    <row customHeight="1" ht="12.75" r="109" s="17"/>
-    <row customHeight="1" ht="12.75" r="110" s="17"/>
-    <row customHeight="1" ht="12.75" r="111" s="17"/>
-    <row customHeight="1" ht="12.75" r="112" s="17"/>
-    <row customHeight="1" ht="12.75" r="113" s="17"/>
-    <row customHeight="1" ht="12.75" r="114" s="17"/>
-    <row customHeight="1" ht="12.75" r="115" s="17"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="95" s="17">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>annesmith</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Anne</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="96" s="17">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>euchariadonnery</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Eucharia</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Donnery</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="97" s="17">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>konstantinakalogirou</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Konstantina</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Kalogirou</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="98" s="17">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>robinreid</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Reid</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="99" s="17">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ninakulovics</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Kulovics</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="100" s="17">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>alinevennemann</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Aline</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Vennemann</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="101" s="17">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>simoneheinkhatib</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Simone</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Hein-Khatib</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="102" s="17">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>marvinschildmeier</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Marvin</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Schildmeier</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="103" s="17">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>barbaraschmenk</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Barbara</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Schmenk</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="104" s="17">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>liligrun</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Lili</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Grün</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="105" s="17">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>richardbale</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Bale</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="106" s="17">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>matthewmichaud</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Michaud</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="107" s="17">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>toddhooper</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Todd</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Hooper</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="108" s="17">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>albabordetas</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Alba</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Bordetas</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="109" s="17">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>yasukoshiozawa</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Yasuko</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Shiozawa</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="110" s="17">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>mihomoody</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Miho</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Moody</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="111" s="17">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>benjaminswakopf</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Swakopf</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="112" s="17">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>dagmarhoffererbrunthaler</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Dagmar</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Höfferer-Brunthaler</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="113" s="17">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>sandrineeschenauer</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Sandrine</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Eschenauer</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="114" s="17">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>ninahasenzagl</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Hasenzagl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="115" s="17">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>annesteiner</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Anne</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Steiner</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+    </row>
     <row customHeight="1" ht="12.75" r="116" s="17"/>
     <row customHeight="1" ht="12.75" r="117" s="17"/>
     <row customHeight="1" ht="12.75" r="118" s="17"/>
@@ -13616,7 +13876,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="25.265625"/>
     <col customWidth="1" max="2" min="2" style="17" width="198.265625"/>
@@ -16234,7 +16494,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="24"/>
     <col customWidth="1" max="26" min="2" style="17" width="8.86328125"/>

</xml_diff>

<commit_message>
fix bug fetching contrib keys
</commit_message>
<xml_diff>
--- a/contribs.xlsx
+++ b/contribs.xlsx
@@ -531,7 +531,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="8.86328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="22.1328125"/>
@@ -1648,7 +1648,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="8.86328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="21.86328125"/>
@@ -2696,7 +2696,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="24"/>
     <col customWidth="1" max="2" min="2" style="17" width="14.59765625"/>
@@ -5810,7 +5810,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="26.1328125"/>
     <col customWidth="1" max="2" min="2" style="17" width="18.3984375"/>
@@ -10611,13 +10611,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="27.06640625"/>
     <col customWidth="1" max="2" min="2" style="17" width="41.19921875"/>
@@ -13098,24 +13098,268 @@
           <t>Steiner</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr"/>
-      <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr"/>
-    </row>
-    <row customHeight="1" ht="12.75" r="116" s="17"/>
-    <row customHeight="1" ht="12.75" r="117" s="17"/>
-    <row customHeight="1" ht="12.75" r="118" s="17"/>
-    <row customHeight="1" ht="12.75" r="119" s="17"/>
-    <row customHeight="1" ht="12.75" r="120" s="17"/>
-    <row customHeight="1" ht="12.75" r="121" s="17"/>
-    <row customHeight="1" ht="12.75" r="122" s="17"/>
-    <row customHeight="1" ht="12.75" r="123" s="17"/>
-    <row customHeight="1" ht="12.75" r="124" s="17"/>
-    <row customHeight="1" ht="12.75" r="125" s="17"/>
-    <row customHeight="1" ht="12.75" r="126" s="17"/>
-    <row customHeight="1" ht="12.75" r="127" s="17"/>
-    <row customHeight="1" ht="12.75" r="128" s="17"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="116" s="17">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>lanesorensen</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Lane</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Sorensen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="117" s="17">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>patriciaklich</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Klich</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="118" s="17">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>maciekklich</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Maciek</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Klich</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.75" r="119" s="17">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>monaeikelpohen</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Mona</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Eikel-Pohen</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="120" s="17">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>leecampbell</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Campbell</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="121" s="17">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>ciarandawson</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Ciarán</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Dawson</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="122" s="17">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>marianmccarthy</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Marian</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>McCarthy</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="123" s="17">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>tomklimant</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Tom</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Klimant</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="124" s="17">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>uschilinehan</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Uschi</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Linehan</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="125" s="17">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>petrabosenius</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Petra</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Bosenius</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="126" s="17">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>susannehorstmann</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Susanne</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Horstmann</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="127" s="17">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>serafinamorrin</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Serafina</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Morrin</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+    </row>
+    <row customHeight="1" ht="12.75" r="128" s="17">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>francescobonelli</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Francesco</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Bonelli</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+    </row>
     <row customHeight="1" ht="12.75" r="129" s="17"/>
     <row customHeight="1" ht="12.75" r="130" s="17"/>
     <row customHeight="1" ht="12.75" r="131" s="17"/>
@@ -13876,7 +14120,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="25.265625"/>
     <col customWidth="1" max="2" min="2" style="17" width="198.265625"/>
@@ -16494,7 +16738,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.3984375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="17" width="24"/>
     <col customWidth="1" max="26" min="2" style="17" width="8.86328125"/>

</xml_diff>

<commit_message>
nice filenames for files; fix titles; fix cover image url
</commit_message>
<xml_diff>
--- a/contribs.xlsx
+++ b/contribs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="3" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="600" firstSheet="3" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Journal" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="_CTVL001f7d0849eae42439cb5fedfc66de80f05" localSheetId="5">#REF!</definedName>
     <definedName name="OLE_LINK24" localSheetId="3">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028" fullCalcOnLoad="1" calcCompleted="0"/>
 </workbook>
 </file>
 
@@ -43,7 +43,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -81,6 +81,17 @@
       <name val="Times New Roman"/>
       <color rgb="FF000000"/>
       <sz val="13"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <i val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <color rgb="FF000000"/>
+      <sz val="6"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -121,9 +132,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -156,6 +167,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -166,7 +178,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,17 +543,17 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="8.86328125" customWidth="1" style="17" min="1" max="1"/>
-    <col width="22.1328125" customWidth="1" style="17" min="2" max="2"/>
+    <col width="8.85546875" customWidth="1" style="17" min="1" max="1"/>
+    <col width="22.140625" customWidth="1" style="17" min="2" max="2"/>
     <col width="20" customWidth="1" style="17" min="3" max="3"/>
-    <col width="26.73046875" customWidth="1" style="17" min="4" max="4"/>
-    <col width="20.73046875" customWidth="1" style="17" min="5" max="5"/>
-    <col width="35.73046875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="26.7109375" customWidth="1" style="17" min="4" max="4"/>
+    <col width="20.7109375" customWidth="1" style="17" min="5" max="5"/>
+    <col width="35.7109375" customWidth="1" style="17" min="6" max="6"/>
     <col width="21" customWidth="1" style="17" min="7" max="7"/>
-    <col width="18.59765625" customWidth="1" style="17" min="8" max="8"/>
-    <col width="8.86328125" customWidth="1" style="17" min="9" max="26"/>
+    <col width="18.5703125" customWidth="1" style="17" min="8" max="8"/>
+    <col width="8.85546875" customWidth="1" style="17" min="9" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="17">
@@ -1648,12 +1660,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="8.86328125" customWidth="1" style="17" min="1" max="1"/>
-    <col width="21.86328125" customWidth="1" style="17" min="2" max="2"/>
-    <col width="15.73046875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="8.86328125" customWidth="1" style="17" min="4" max="26"/>
+    <col width="8.85546875" customWidth="1" style="17" min="1" max="1"/>
+    <col width="21.85546875" customWidth="1" style="17" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="17" min="3" max="3"/>
+    <col width="8.85546875" customWidth="1" style="17" min="4" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="17">
@@ -2696,17 +2708,17 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="24" customWidth="1" style="17" min="1" max="1"/>
-    <col width="14.59765625" customWidth="1" style="17" min="2" max="2"/>
-    <col width="12.1328125" customWidth="1" style="17" min="3" max="3"/>
-    <col width="22.73046875" customWidth="1" style="17" min="4" max="4"/>
-    <col width="15.1328125" customWidth="1" style="17" min="5" max="5"/>
-    <col width="52.73046875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="24.1328125" customWidth="1" style="17" min="7" max="7"/>
-    <col width="24.59765625" customWidth="1" style="17" min="8" max="8"/>
-    <col width="8.86328125" customWidth="1" style="17" min="9" max="26"/>
+    <col width="14.5703125" customWidth="1" style="17" min="2" max="2"/>
+    <col width="12.140625" customWidth="1" style="17" min="3" max="3"/>
+    <col width="22.7109375" customWidth="1" style="17" min="4" max="4"/>
+    <col width="15.140625" customWidth="1" style="17" min="5" max="5"/>
+    <col width="52.7109375" customWidth="1" style="17" min="6" max="6"/>
+    <col width="24.140625" customWidth="1" style="17" min="7" max="7"/>
+    <col width="24.5703125" customWidth="1" style="17" min="8" max="8"/>
+    <col width="8.85546875" customWidth="1" style="17" min="9" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="17">
@@ -2773,7 +2785,7 @@
       <c r="E2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="inlineStr">
+      <c r="F2" s="19" t="inlineStr">
         <is>
           <t>http://research.ucc.ie/scenario/2020/01</t>
         </is>
@@ -5806,28 +5818,28 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="26.1328125" customWidth="1" style="17" min="1" max="1"/>
-    <col width="18.3984375" customWidth="1" style="17" min="2" max="2"/>
-    <col width="92.3984375" customWidth="1" style="17" min="3" max="3"/>
-    <col width="42.86328125" customWidth="1" style="17" min="4" max="4"/>
-    <col width="51.86328125" customWidth="1" style="17" min="5" max="5"/>
-    <col width="41.86328125" customWidth="1" style="17" min="6" max="6"/>
-    <col width="22.73046875" customWidth="1" style="17" min="7" max="7"/>
-    <col width="66.59765625" customWidth="1" style="17" min="8" max="8"/>
-    <col width="33.3984375" customWidth="1" style="17" min="9" max="10"/>
-    <col width="22.59765625" customWidth="1" style="17" min="11" max="11"/>
-    <col width="21.1328125" customWidth="1" style="17" min="12" max="12"/>
-    <col width="92.86328125" customWidth="1" style="17" min="13" max="13"/>
-    <col width="29.73046875" customWidth="1" style="17" min="14" max="14"/>
-    <col width="29.265625" customWidth="1" style="17" min="15" max="15"/>
-    <col width="37.1328125" customWidth="1" style="17" min="16" max="16"/>
-    <col width="170.1328125" customWidth="1" style="17" min="17" max="17"/>
+    <col width="26.140625" customWidth="1" style="17" min="1" max="1"/>
+    <col width="18.42578125" customWidth="1" style="17" min="2" max="2"/>
+    <col width="92.42578125" customWidth="1" style="17" min="3" max="3"/>
+    <col width="42.85546875" customWidth="1" style="17" min="4" max="4"/>
+    <col width="51.85546875" customWidth="1" style="17" min="5" max="5"/>
+    <col width="41.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="22.7109375" customWidth="1" style="17" min="7" max="7"/>
+    <col width="66.5703125" customWidth="1" style="17" min="8" max="8"/>
+    <col width="33.42578125" customWidth="1" style="17" min="9" max="10"/>
+    <col width="22.5703125" customWidth="1" style="17" min="11" max="11"/>
+    <col width="21.140625" customWidth="1" style="17" min="12" max="12"/>
+    <col width="92.85546875" customWidth="1" style="17" min="13" max="13"/>
+    <col width="29.7109375" customWidth="1" style="17" min="14" max="14"/>
+    <col width="29.28515625" customWidth="1" style="17" min="15" max="15"/>
+    <col width="37.140625" customWidth="1" style="17" min="16" max="16"/>
+    <col width="170.140625" customWidth="1" style="17" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="17">
@@ -5951,7 +5963,7 @@
       <c r="G2" s="3" t="n">
         <v>44015</v>
       </c>
-      <c r="H2" s="22" t="inlineStr">
+      <c r="H2" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">http://research.ucc.ie/scenario/2020/01/FOREWORD/00/en </t>
         </is>
@@ -6299,7 +6311,7 @@
       <c r="G8" s="3" t="n">
         <v>44015</v>
       </c>
-      <c r="H8" s="19" t="inlineStr">
+      <c r="H8" s="20" t="inlineStr">
         <is>
           <t>http://research.ucc.ie/journals/scenario/2020/01/ARTS/06/en</t>
         </is>
@@ -10613,20 +10625,20 @@
   </sheetPr>
   <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="27.06640625" customWidth="1" style="17" min="1" max="1"/>
-    <col width="41.19921875" customWidth="1" style="17" min="2" max="2"/>
-    <col width="36.19921875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="23.59765625" customWidth="1" style="17" min="4" max="4"/>
-    <col width="32.1328125" customWidth="1" style="17" min="5" max="5"/>
+    <col width="8.28515625" customWidth="1" style="17" min="1" max="1"/>
+    <col width="11.7109375" customWidth="1" style="17" min="2" max="2"/>
+    <col width="16.7109375" customWidth="1" style="17" min="3" max="3"/>
+    <col width="23.5703125" customWidth="1" style="17" min="4" max="4"/>
+    <col width="32.140625" customWidth="1" style="17" min="5" max="5"/>
     <col width="32" customWidth="1" style="17" min="6" max="6"/>
-    <col width="25.86328125" customWidth="1" style="17" min="7" max="7"/>
-    <col width="8.86328125" customWidth="1" style="17" min="8" max="26"/>
+    <col width="25.85546875" customWidth="1" style="17" min="7" max="7"/>
+    <col width="8.85546875" customWidth="1" style="17" min="8" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="17">
@@ -11566,7 +11578,7 @@
           <t>Berlin University of the Arts</t>
         </is>
       </c>
-      <c r="G34" s="20" t="inlineStr">
+      <c r="G34" s="21" t="inlineStr">
         <is>
           <t>uhen@udk-berlin.de</t>
         </is>
@@ -11821,7 +11833,7 @@
           <t>Dufeu</t>
         </is>
       </c>
-      <c r="G44" s="22" t="inlineStr">
+      <c r="G44" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">dufeu@psychodramaturgie.org  </t>
         </is>
@@ -11848,7 +11860,7 @@
           <t>Rikkyo University Tokyo, Japan</t>
         </is>
       </c>
-      <c r="G45" s="22" t="inlineStr">
+      <c r="G45" s="23" t="inlineStr">
         <is>
           <t>nfor.samuel@rikkyo.ac.jp</t>
         </is>
@@ -11875,7 +11887,7 @@
           <t>Ludwig-Maximilians-University, Munich</t>
         </is>
       </c>
-      <c r="G46" s="22" t="inlineStr">
+      <c r="G46" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">katrin.geneuss@germanistik.uni-muenchen.de   </t>
         </is>
@@ -11902,7 +11914,7 @@
           <t>Ludwig-Maximilians-University, Munich</t>
         </is>
       </c>
-      <c r="G47" s="22" t="inlineStr">
+      <c r="G47" s="23" t="inlineStr">
         <is>
           <t>fabian.obster@stablab.stat.uni-muenchen.de</t>
         </is>
@@ -11924,7 +11936,7 @@
           <t>Ruppert</t>
         </is>
       </c>
-      <c r="G48" s="22" t="inlineStr">
+      <c r="G48" s="23" t="inlineStr">
         <is>
           <t>g.ruppert@campus.lmu.de</t>
         </is>
@@ -11951,7 +11963,7 @@
           <t xml:space="preserve">King’s College London </t>
         </is>
       </c>
-      <c r="G49" s="22" t="inlineStr">
+      <c r="G49" s="23" t="inlineStr">
         <is>
           <t>angelique.arts@kcl.ac.uk</t>
         </is>
@@ -11978,7 +11990,7 @@
           <t>O.P. Jindal Global University</t>
         </is>
       </c>
-      <c r="G50" s="22" t="inlineStr">
+      <c r="G50" s="23" t="inlineStr">
         <is>
           <t>shruti@jgu.edu.in</t>
         </is>
@@ -12005,7 +12017,7 @@
           <t>Konstanz University of Applied Sciences</t>
         </is>
       </c>
-      <c r="G51" s="22" t="inlineStr">
+      <c r="G51" s="23" t="inlineStr">
         <is>
           <t>stefanie.giebert@mail.de</t>
         </is>
@@ -12048,483 +12060,483 @@
     <row r="54" ht="12.75" customHeight="1" s="17">
       <c r="A54" t="inlineStr">
         <is>
-          <t>mariagiovannabiscu</t>
+          <t>shereeborge</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Maria Giovanna</t>
+          <t>Sheree</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Biscu</t>
+          <t>Borge</t>
         </is>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1" s="17">
       <c r="A55" t="inlineStr">
         <is>
-          <t>mariaisabelfernandesgarcia</t>
+          <t>annaweiss</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>María Isabel</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Fernándes García</t>
+          <t>Weiss</t>
         </is>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1" s="17">
       <c r="A56" t="inlineStr">
         <is>
-          <t>michaeljsosulski</t>
+          <t>bettinamatthias</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Michael J.</t>
+          <t>Bettina</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Sosulski</t>
+          <t>Matthias</t>
         </is>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1" s="17">
       <c r="A57" t="inlineStr">
         <is>
-          <t>grahamwlea</t>
+          <t>ulrichwettemann</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Graham W.</t>
+          <t>Ulrich</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Lea</t>
+          <t>Wettemann</t>
         </is>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1" s="17">
       <c r="A58" t="inlineStr">
         <is>
-          <t>kellyckingsbury</t>
+          <t>ulrikebrisson</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kelly C.</t>
+          <t>Ulrike</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Kingsbury</t>
+          <t>Brisson</t>
         </is>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1" s="17">
       <c r="A59" t="inlineStr">
         <is>
-          <t>lynnmariekutch</t>
+          <t>mariaeisenmann</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lynn Marie</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Kutch</t>
+          <t>Eisenmann</t>
         </is>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1" s="17">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ursulachristinebunger</t>
+          <t>christianelutge</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ursula Christine</t>
+          <t>Christiane</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Bünger</t>
+          <t>Lütge</t>
         </is>
       </c>
     </row>
     <row r="61" ht="12.75" customHeight="1" s="17">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sabinavecchionegruner</t>
+          <t>birgitoelschlager</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sabina</t>
+          <t>Birgit</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Vecchione Grüner</t>
+          <t>Oelschläger</t>
         </is>
       </c>
     </row>
     <row r="62" ht="12.75" customHeight="1" s="17">
       <c r="A62" t="inlineStr">
         <is>
-          <t>erikamnelson</t>
+          <t>christophransmayr</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Erika M.</t>
+          <t>Christoph</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Nelson</t>
+          <t>Ransmayr</t>
         </is>
       </c>
     </row>
     <row r="63" ht="12.75" customHeight="1" s="17">
       <c r="A63" t="inlineStr">
         <is>
-          <t>mariaisabelfernandezgarcia</t>
+          <t>mercedesariza</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>María Isabel</t>
+          <t>Mercedes</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Fernández García</t>
+          <t>Ariza</t>
         </is>
       </c>
     </row>
     <row r="64" ht="12.75" customHeight="1" s="17">
       <c r="A64" t="inlineStr">
         <is>
-          <t>anturomeronunes</t>
+          <t>mariagiovannabiscu</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Antu Romero</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Nunes</t>
+          <t>Giovanna Biscu</t>
         </is>
       </c>
     </row>
     <row r="65" ht="12.75" customHeight="1" s="17">
       <c r="A65" t="inlineStr">
         <is>
-          <t>maxpeterammann</t>
+          <t>mariaisabelfernandesgarcia</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Max Peter</t>
+          <t>María</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Ammann</t>
+          <t>Isabel Fernándes García</t>
         </is>
       </c>
     </row>
     <row r="66" ht="12.75" customHeight="1" s="17">
       <c r="A66" t="inlineStr">
         <is>
-          <t>leticiagarciabrea</t>
+          <t>alexandrazimmermann</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Leticia</t>
+          <t>Alexandra</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>García Brea</t>
+          <t>Zimmermann</t>
         </is>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1" s="17">
       <c r="A67" t="inlineStr">
         <is>
-          <t>isobelniriain</t>
+          <t>danielfeldhendler</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Isobel</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Ní Riain</t>
+          <t>Feldhendler</t>
         </is>
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1" s="17">
       <c r="A68" t="inlineStr">
         <is>
-          <t>sophiecharlotterummel</t>
+          <t>stefanhajduk</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sophie Charlotte</t>
+          <t>Stefan</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Rummel</t>
+          <t>Hajduk</t>
         </is>
       </c>
     </row>
     <row r="69" ht="12.75" customHeight="1" s="17">
       <c r="A69" t="inlineStr">
         <is>
-          <t>amirhosseinesmkhani</t>
+          <t>chrisritchie</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Amir Hossein</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Esmkhani</t>
+          <t>Ritchie</t>
         </is>
       </c>
     </row>
     <row r="70" ht="12.75" customHeight="1" s="17">
       <c r="A70" t="inlineStr">
         <is>
-          <t>kathleenrosemcgovern</t>
+          <t>jamesharris</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Kathleen Rose</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>McGovern</t>
+          <t>Harris</t>
         </is>
       </c>
     </row>
     <row r="71" ht="12.75" customHeight="1" s="17">
       <c r="A71" t="inlineStr">
         <is>
-          <t>catherinevanhalsema</t>
+          <t>barbeljogschies</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Catherine</t>
+          <t>Bärbel</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Van Halsema</t>
+          <t>Jogschies</t>
         </is>
       </c>
     </row>
     <row r="72" ht="12.75" customHeight="1" s="17">
       <c r="A72" t="inlineStr">
         <is>
-          <t>gustavejweltsek</t>
+          <t>peterjankowsky</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Gustave J.</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Weltsek</t>
+          <t>Jankowsky</t>
         </is>
       </c>
     </row>
     <row r="73" ht="12.75" customHeight="1" s="17">
       <c r="A73" t="inlineStr">
         <is>
-          <t>michaelklegutke</t>
+          <t>michaeljsosulski</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Michael K.</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Legutke</t>
+          <t>J. Sosulski</t>
         </is>
       </c>
     </row>
     <row r="74" ht="12.75" customHeight="1" s="17">
       <c r="A74" t="inlineStr">
         <is>
-          <t>konstantinosprokopiostrimmis</t>
+          <t>marklauer</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Konstantinos Prokopios</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Trimmis</t>
+          <t>Lauer</t>
         </is>
       </c>
     </row>
     <row r="75" ht="12.75" customHeight="1" s="17">
       <c r="A75" t="inlineStr">
         <is>
-          <t>johncrutchfield</t>
+          <t>steffiretzlaff</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Steffi</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Crutchfield</t>
+          <t>Retzlaff</t>
         </is>
       </c>
     </row>
     <row r="76" ht="12.75" customHeight="1" s="17">
       <c r="A76" t="inlineStr">
         <is>
-          <t>bokjacho</t>
+          <t>frankfischass</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Bokja</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Cho</t>
+          <t>Fischäss</t>
         </is>
       </c>
     </row>
     <row r="77" ht="12.75" customHeight="1" s="17">
       <c r="A77" t="inlineStr">
         <is>
-          <t>martinaturecek</t>
+          <t>marinabertino</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Martina</t>
+          <t>Marina</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Turecek</t>
+          <t>Bertino</t>
         </is>
       </c>
     </row>
     <row r="78" ht="12.75" customHeight="1" s="17">
       <c r="A78" t="inlineStr">
         <is>
-          <t>philippbotes</t>
+          <t>frankmccourt</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Philipp</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Botes</t>
+          <t>McCourt</t>
         </is>
       </c>
     </row>
     <row r="79" ht="12.75" customHeight="1" s="17">
       <c r="A79" t="inlineStr">
         <is>
-          <t>danielberghoff</t>
+          <t>benediktkessler</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Benedikt</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Berghoff</t>
+          <t>Kessler</t>
         </is>
       </c>
     </row>
     <row r="80" ht="12.75" customHeight="1" s="17">
       <c r="A80" t="inlineStr">
         <is>
-          <t>peadardonohoe</t>
+          <t>almutkuppers</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Peadar</t>
+          <t>Almut</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Donohoe</t>
+          <t>Küppers</t>
         </is>
       </c>
     </row>
     <row r="81" ht="12.75" customHeight="1" s="17">
       <c r="A81" t="inlineStr">
         <is>
-          <t>hanneseitz</t>
+          <t>nathaliefratini</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Hanne</t>
+          <t>Nathalie</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Seitz</t>
+          <t>Fratini</t>
         </is>
       </c>
     </row>
     <row r="82" ht="12.75" customHeight="1" s="17">
       <c r="A82" t="inlineStr">
         <is>
-          <t>kristinwestphal</t>
+          <t>kristinwardetzky</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -12534,2756 +12546,2756 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Westphal</t>
+          <t>Wardetzky</t>
         </is>
       </c>
     </row>
     <row r="83" ht="12.75" customHeight="1" s="17">
       <c r="A83" t="inlineStr">
         <is>
-          <t>sabinedengscherz</t>
+          <t>christianeweigel</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sabine</t>
+          <t>Christiane</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Dengscherz</t>
+          <t>Weigel</t>
         </is>
       </c>
     </row>
     <row r="84" ht="12.75" customHeight="1" s="17">
       <c r="A84" t="inlineStr">
         <is>
-          <t>stefaniebeckmann</t>
+          <t>jennypasson</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Stefanie</t>
+          <t>Jenny</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Beckmann</t>
+          <t>Passon</t>
         </is>
       </c>
     </row>
     <row r="85" ht="12.75" customHeight="1" s="17">
       <c r="A85" t="inlineStr">
         <is>
-          <t>doreenbryant</t>
+          <t>joachimbeug</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Doreen</t>
+          <t>Joachim</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Bryant</t>
+          <t>Beug</t>
         </is>
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1" s="17">
       <c r="A86" t="inlineStr">
         <is>
-          <t>jonathansharp</t>
+          <t>gottfriedkeller</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Gottfried</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Sharp</t>
+          <t>Keller</t>
         </is>
       </c>
     </row>
     <row r="87" ht="12.75" customHeight="1" s="17">
       <c r="A87" t="inlineStr">
         <is>
-          <t>angelikailg</t>
+          <t>doriskrohn</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Angelika</t>
+          <t>Doris</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Ilg</t>
+          <t>Krohn</t>
         </is>
       </c>
     </row>
     <row r="88" ht="12.75" customHeight="1" s="17">
       <c r="A88" t="inlineStr">
         <is>
-          <t>sabinekutzelmann</t>
+          <t>euchariadonnery</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Sabine</t>
+          <t>Eucharia</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Kutzelmann</t>
+          <t>Donnery</t>
         </is>
       </c>
     </row>
     <row r="89" ht="12.75" customHeight="1" s="17">
       <c r="A89" t="inlineStr">
         <is>
-          <t>utemassler</t>
+          <t>seanaita</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Ute</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Massler</t>
+          <t>Aita</t>
         </is>
       </c>
     </row>
     <row r="90" ht="12.75" customHeight="1" s="17">
       <c r="A90" t="inlineStr">
         <is>
-          <t>klauspeter</t>
+          <t>astridlindgren</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Klaus</t>
+          <t>Astrid</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Peter</t>
+          <t>Lindgren</t>
         </is>
       </c>
     </row>
     <row r="91" ht="12.75" customHeight="1" s="17">
       <c r="A91" t="inlineStr">
         <is>
-          <t>kerstintheinert</t>
+          <t>utaschorlemmer</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Kerstin</t>
+          <t>Uta</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Theinert</t>
+          <t>Schorlemmer</t>
         </is>
       </c>
     </row>
     <row r="92" ht="12.75" customHeight="1" s="17">
       <c r="A92" t="inlineStr">
         <is>
-          <t>michaelareinhardt</t>
+          <t>barbarasinisi</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Michaela</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Reinhardt</t>
+          <t>Sinisi</t>
         </is>
       </c>
     </row>
     <row r="93" ht="12.75" customHeight="1" s="17">
       <c r="A93" t="inlineStr">
         <is>
-          <t>umbertocapra</t>
+          <t>amandawager</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Umberto</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Capra</t>
+          <t>Wager</t>
         </is>
       </c>
     </row>
     <row r="94" ht="12.75" customHeight="1" s="17">
       <c r="A94" t="inlineStr">
         <is>
-          <t>abigailpaul</t>
+          <t>georgebelliveau</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Abigail</t>
+          <t>George</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Belliveau</t>
         </is>
       </c>
     </row>
     <row r="95" ht="12.75" customHeight="1" s="17">
       <c r="A95" t="inlineStr">
         <is>
-          <t>shereeborge</t>
+          <t>jaimebeck</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Sheree</t>
+          <t>Jaime</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Borge</t>
+          <t>Beck</t>
         </is>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1" s="17">
       <c r="A96" t="inlineStr">
         <is>
-          <t>annaweiss</t>
+          <t>grahamwlea</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Weiss</t>
+          <t>W. Lea</t>
         </is>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1" s="17">
       <c r="A97" t="inlineStr">
         <is>
-          <t>bettinamatthias</t>
+          <t>christianschmittkilb</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Bettina</t>
+          <t>Christian</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Matthias</t>
+          <t>Schmitt-Kilb</t>
         </is>
       </c>
     </row>
     <row r="98" ht="12.75" customHeight="1" s="17">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ulrichwettemann</t>
+          <t>kellyckingsbury</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Ulrich</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Wettemann</t>
+          <t>C. Kingsbury</t>
         </is>
       </c>
     </row>
     <row r="99" ht="12.75" customHeight="1" s="17">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ulrikebrisson</t>
+          <t>wolfganghallet</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Ulrike</t>
+          <t>Wolfgang</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Brisson</t>
+          <t>Hallet</t>
         </is>
       </c>
     </row>
     <row r="100" ht="12.75" customHeight="1" s="17">
       <c r="A100" t="inlineStr">
         <is>
-          <t>mariaeisenmann</t>
+          <t>heikewedel</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Heike</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Eisenmann</t>
+          <t>Wedel</t>
         </is>
       </c>
     </row>
     <row r="101" ht="12.75" customHeight="1" s="17">
       <c r="A101" t="inlineStr">
         <is>
-          <t>christianelutge</t>
+          <t>adrianhaack</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Christiane</t>
+          <t>Adrian</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Lütge</t>
+          <t>Haack</t>
         </is>
       </c>
     </row>
     <row r="102" ht="12.75" customHeight="1" s="17">
       <c r="A102" t="inlineStr">
         <is>
-          <t>birgitoelschlager</t>
+          <t>renatacieslak</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Birgit</t>
+          <t>Renata</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Oelschläger</t>
+          <t>Cieslak</t>
         </is>
       </c>
     </row>
     <row r="103" ht="12.75" customHeight="1" s="17">
       <c r="A103" t="inlineStr">
         <is>
-          <t>christophransmayr</t>
+          <t>theodorstorm</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Christoph</t>
+          <t>Theodor</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Ransmayr</t>
+          <t>Storm</t>
         </is>
       </c>
     </row>
     <row r="104" ht="12.75" customHeight="1" s="17">
       <c r="A104" t="inlineStr">
         <is>
-          <t>mercedesariza</t>
+          <t>lynnmariekutch</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Mercedes</t>
+          <t>Lynn</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Ariza</t>
+          <t>Marie Kutch</t>
         </is>
       </c>
     </row>
     <row r="105" ht="12.75" customHeight="1" s="17">
       <c r="A105" t="inlineStr">
         <is>
-          <t>alexandrazimmermann</t>
+          <t>ursulachristinebunger</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Alexandra</t>
+          <t>Ursula</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Zimmermann</t>
+          <t>Christine Bünger</t>
         </is>
       </c>
     </row>
     <row r="106" ht="12.75" customHeight="1" s="17">
       <c r="A106" t="inlineStr">
         <is>
-          <t>danielfeldhendler</t>
+          <t>stephenboyd</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Stephen</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Feldhendler</t>
+          <t>Boyd</t>
         </is>
       </c>
     </row>
     <row r="107" ht="12.75" customHeight="1" s="17">
       <c r="A107" t="inlineStr">
         <is>
-          <t>stefanhajduk</t>
+          <t>michaelende</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Stefan</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Hajduk</t>
+          <t>Ende</t>
         </is>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" s="17">
       <c r="A108" t="inlineStr">
         <is>
-          <t>chrisritchie</t>
+          <t>fionadalziel</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Fiona</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Ritchie</t>
+          <t>Dalziel</t>
         </is>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" s="17">
       <c r="A109" t="inlineStr">
         <is>
-          <t>jamesharris</t>
+          <t>annasantucci</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Santucci</t>
         </is>
       </c>
     </row>
     <row r="110" ht="12.75" customHeight="1" s="17">
       <c r="A110" t="inlineStr">
         <is>
-          <t>barbeljogschies</t>
+          <t>giampaolospedo</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Bärbel</t>
+          <t>Giampaolo</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Jogschies</t>
+          <t>Spedo</t>
         </is>
       </c>
     </row>
     <row r="111" ht="12.75" customHeight="1" s="17">
       <c r="A111" t="inlineStr">
         <is>
-          <t>peterjankowsky</t>
+          <t>brigittehahnmichaeli</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Peter</t>
+          <t>Brigitte</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Jankowsky</t>
+          <t>Hahn-Michaeli</t>
         </is>
       </c>
     </row>
     <row r="112" ht="12.75" customHeight="1" s="17">
       <c r="A112" t="inlineStr">
         <is>
-          <t>marklauer</t>
+          <t>baradockalova</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bara</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Lauer</t>
+          <t>Dockalova</t>
         </is>
       </c>
     </row>
     <row r="113" ht="12.75" customHeight="1" s="17">
       <c r="A113" t="inlineStr">
         <is>
-          <t>steffiretzlaff</t>
+          <t>barbaraschmenk</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Steffi</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Retzlaff</t>
+          <t>Schmenk</t>
         </is>
       </c>
     </row>
     <row r="114" ht="12.75" customHeight="1" s="17">
       <c r="A114" t="inlineStr">
         <is>
-          <t>frankfischass</t>
+          <t>marynoonan</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Fischäss</t>
+          <t>Noonan</t>
         </is>
       </c>
     </row>
     <row r="115" ht="12.75" customHeight="1" s="17">
       <c r="A115" t="inlineStr">
         <is>
-          <t>marinabertino</t>
+          <t>fromfaustbyjohannwolfgangvongoethe</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Marina</t>
+          <t>from:</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Bertino</t>
+          <t>FAUST by Johann Wolfgang von Goethe</t>
         </is>
       </c>
     </row>
     <row r="116" ht="12.75" customHeight="1" s="17">
       <c r="A116" t="inlineStr">
         <is>
-          <t>frankmccourt</t>
+          <t>eddaholl</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Edda</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>McCourt</t>
+          <t>Holl</t>
         </is>
       </c>
     </row>
     <row r="117" ht="12.75" customHeight="1" s="17">
       <c r="A117" t="inlineStr">
         <is>
-          <t>benediktkessler</t>
+          <t>giselafasse</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Benedikt</t>
+          <t>Gisela</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Kessler</t>
+          <t>Fasse</t>
         </is>
       </c>
     </row>
     <row r="118" ht="12.75" customHeight="1" s="17">
       <c r="A118" t="inlineStr">
         <is>
-          <t>almutkuppers</t>
+          <t>sabinavecchionegruner</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Almut</t>
+          <t>Sabina</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Küppers</t>
+          <t>Vecchione Grüner</t>
         </is>
       </c>
     </row>
     <row r="119" ht="12.75" customHeight="1" s="17">
       <c r="A119" t="inlineStr">
         <is>
-          <t>nathaliefratini</t>
+          <t>sigridunterstab</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Nathalie</t>
+          <t>Sigrid</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Fratini</t>
+          <t>Unterstab</t>
         </is>
       </c>
     </row>
     <row r="120" ht="12.75" customHeight="1" s="17">
       <c r="A120" t="inlineStr">
         <is>
-          <t>kristinwardetzky</t>
+          <t>siegfriedboehm</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Kristin</t>
+          <t>Siegfried</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Wardetzky</t>
+          <t>Boehm</t>
         </is>
       </c>
     </row>
     <row r="121" ht="12.75" customHeight="1" s="17">
       <c r="A121" t="inlineStr">
         <is>
-          <t>christianeweigel</t>
+          <t>filippofonio</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Christiane</t>
+          <t>Filippo</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Weigel</t>
+          <t>Fonio</t>
         </is>
       </c>
     </row>
     <row r="122" ht="12.75" customHeight="1" s="17">
       <c r="A122" t="inlineStr">
         <is>
-          <t>jennypasson</t>
+          <t>genevievegenicot</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Jenny</t>
+          <t>Geneviève</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Passon</t>
+          <t>Genicot</t>
         </is>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" s="17">
       <c r="A123" t="inlineStr">
         <is>
-          <t>joachimbeug</t>
+          <t>erikamnelson</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Joachim</t>
+          <t>Erika</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Beug</t>
+          <t>M. Nelson</t>
         </is>
       </c>
     </row>
     <row r="124" ht="12.75" customHeight="1" s="17">
       <c r="A124" t="inlineStr">
         <is>
-          <t>gottfriedkeller</t>
+          <t>renatebreitig</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Gottfried</t>
+          <t>Renate</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Keller</t>
+          <t>Breitig</t>
         </is>
       </c>
     </row>
     <row r="125" ht="12.75" customHeight="1" s="17">
       <c r="A125" t="inlineStr">
         <is>
-          <t>doriskrohn</t>
+          <t>christianegunther</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Doris</t>
+          <t>Christiane</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Krohn</t>
+          <t>Günther</t>
         </is>
       </c>
     </row>
     <row r="126" ht="12.75" customHeight="1" s="17">
       <c r="A126" t="inlineStr">
         <is>
-          <t>euchariadonnery</t>
+          <t>racheldarby</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Eucharia</t>
+          <t>Rachel</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Donnery</t>
+          <t>Darby</t>
         </is>
       </c>
     </row>
     <row r="127" ht="12.75" customHeight="1" s="17">
       <c r="A127" t="inlineStr">
         <is>
-          <t>seanaita</t>
+          <t>doreenbryant</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Doreen</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Aita</t>
+          <t>Bryant</t>
         </is>
       </c>
     </row>
     <row r="128" ht="12.75" customHeight="1" s="17">
       <c r="A128" t="inlineStr">
         <is>
-          <t>astridlindgren</t>
+          <t>wolfgangsting</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Astrid</t>
+          <t>Wolfgang</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Lindgren</t>
+          <t>Sting</t>
         </is>
       </c>
     </row>
     <row r="129" ht="12.75" customHeight="1" s="17">
       <c r="A129" t="inlineStr">
         <is>
-          <t>utaschorlemmer</t>
+          <t>juliakinze</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Uta</t>
+          <t>Julia</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Schorlemmer</t>
+          <t>Kinze</t>
         </is>
       </c>
     </row>
     <row r="130" ht="12.75" customHeight="1" s="17">
       <c r="A130" t="inlineStr">
         <is>
-          <t>barbarasinisi</t>
+          <t>romidomkowsky</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Romi</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Sinisi</t>
+          <t>Domkowsky</t>
         </is>
       </c>
     </row>
     <row r="131" ht="12.75" customHeight="1" s="17">
       <c r="A131" t="inlineStr">
         <is>
-          <t>amandawager</t>
+          <t>michafleiner</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Micha</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Wager</t>
+          <t>Fleiner</t>
         </is>
       </c>
     </row>
     <row r="132" ht="12.75" customHeight="1" s="17">
       <c r="A132" t="inlineStr">
         <is>
-          <t>georgebelliveau</t>
+          <t>nicolettamarinimaio</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Nicoletta</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Belliveau</t>
+          <t>Marini-Maio</t>
         </is>
       </c>
     </row>
     <row r="133" ht="12.75" customHeight="1" s="17">
       <c r="A133" t="inlineStr">
         <is>
-          <t>jaimebeck</t>
+          <t>andreapennacchi</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Jaime</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Beck</t>
+          <t>Pennacchi</t>
         </is>
       </c>
     </row>
     <row r="134" ht="12.75" customHeight="1" s="17">
       <c r="A134" t="inlineStr">
         <is>
-          <t>christianschmittkilb</t>
+          <t>lornacarson</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Christian</t>
+          <t>Lorna</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Schmitt-Kilb</t>
+          <t>Carson</t>
         </is>
       </c>
     </row>
     <row r="135" ht="12.75" customHeight="1" s="17">
       <c r="A135" t="inlineStr">
         <is>
-          <t>wolfganghallet</t>
+          <t>ivanlombardi</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Wolfgang</t>
+          <t>Ivan</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Hallet</t>
+          <t>Lombardi</t>
         </is>
       </c>
     </row>
     <row r="136" ht="12.75" customHeight="1" s="17">
       <c r="A136" t="inlineStr">
         <is>
-          <t>heikewedel</t>
+          <t>mariaisabelfernandezgarcia</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Heike</t>
+          <t>María</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Wedel</t>
+          <t>Isabel Fernández García</t>
         </is>
       </c>
     </row>
     <row r="137" ht="12.75" customHeight="1" s="17">
       <c r="A137" t="inlineStr">
         <is>
-          <t>adrianhaack</t>
+          <t>claudiobendazzoli</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Adrian</t>
+          <t>Claudio</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Haack</t>
+          <t>Bendazzoli</t>
         </is>
       </c>
     </row>
     <row r="138" ht="12.75" customHeight="1" s="17">
       <c r="A138" t="inlineStr">
         <is>
-          <t>renatacieslak</t>
+          <t>yvonnegrimaldi</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Renata</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Cieslak</t>
+          <t>Grimaldi</t>
         </is>
       </c>
     </row>
     <row r="139" ht="12.75" customHeight="1" s="17">
       <c r="A139" t="inlineStr">
         <is>
-          <t>theodorstorm</t>
+          <t>gabriellacaponidoherty</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Theodor</t>
+          <t>Gabriella</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Storm</t>
+          <t>Caponi-Doherty</t>
         </is>
       </c>
     </row>
     <row r="140" ht="12.75" customHeight="1" s="17">
       <c r="A140" t="inlineStr">
         <is>
-          <t>stephenboyd</t>
+          <t>jensulrichdavids</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Stephen</t>
+          <t>Jens-Ulrich</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Boyd</t>
+          <t>Davids</t>
         </is>
       </c>
     </row>
     <row r="141" ht="12.75" customHeight="1" s="17">
       <c r="A141" t="inlineStr">
         <is>
-          <t>michaelende</t>
+          <t>karelzdarek</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Karel</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Ende</t>
+          <t>Zdarek</t>
         </is>
       </c>
     </row>
     <row r="142" ht="12.75" customHeight="1" s="17">
       <c r="A142" t="inlineStr">
         <is>
-          <t>fionadalziel</t>
+          <t>theresabirnbaum</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Fiona</t>
+          <t>Theresa</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Dalziel</t>
+          <t>Birnbaum</t>
         </is>
       </c>
     </row>
     <row r="143" ht="12.75" customHeight="1" s="17">
       <c r="A143" t="inlineStr">
         <is>
-          <t>annasantucci</t>
+          <t>michaelasambanis</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Michaela</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Santucci</t>
+          <t>Sambanis</t>
         </is>
       </c>
     </row>
     <row r="144" ht="12.75" customHeight="1" s="17">
       <c r="A144" t="inlineStr">
         <is>
-          <t>giampaolospedo</t>
+          <t>delilbaran</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Giampaolo</t>
+          <t>Delil</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Spedo</t>
+          <t>Baran</t>
         </is>
       </c>
     </row>
     <row r="145" ht="12.75" customHeight="1" s="17">
       <c r="A145" t="inlineStr">
         <is>
-          <t>brigittehahnmichaeli</t>
+          <t>kimonbeltrop</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Brigitte</t>
+          <t>Kimon</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Hahn-Michaeli</t>
+          <t>Beltrop</t>
         </is>
       </c>
     </row>
     <row r="146" ht="12.75" customHeight="1" s="17">
       <c r="A146" t="inlineStr">
         <is>
-          <t>baradockalova</t>
+          <t>lisagrabert</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Bara</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Dockalova</t>
+          <t>Grabert</t>
         </is>
       </c>
     </row>
     <row r="147" ht="12.75" customHeight="1" s="17">
       <c r="A147" t="inlineStr">
         <is>
-          <t>barbaraschmenk</t>
+          <t>janinaknorrdadfar</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Janina</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Schmenk</t>
+          <t>Knorr-Dadfar</t>
         </is>
       </c>
     </row>
     <row r="148" ht="12.75" customHeight="1" s="17">
       <c r="A148" t="inlineStr">
         <is>
-          <t>marynoonan</t>
+          <t>josephinmarz</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Josephin</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Noonan</t>
+          <t>März</t>
         </is>
       </c>
     </row>
     <row r="149" ht="12.75" customHeight="1" s="17">
       <c r="A149" t="inlineStr">
         <is>
-          <t>fromfaustbyjohannwolfgangvongoethe</t>
+          <t>andreaschneider</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>from:</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>FAUST by Johann Wolfgang von Goethe</t>
+          <t>Schneider</t>
         </is>
       </c>
     </row>
     <row r="150" ht="12.75" customHeight="1" s="17">
       <c r="A150" t="inlineStr">
         <is>
-          <t>eddaholl</t>
+          <t>franksplitt</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Edda</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Holl</t>
+          <t>Splitt</t>
         </is>
       </c>
     </row>
     <row r="151" ht="12.75" customHeight="1" s="17">
       <c r="A151" t="inlineStr">
         <is>
-          <t>giselafasse</t>
+          <t>katharinawonschik</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Gisela</t>
+          <t>Katharina</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Fasse</t>
+          <t>Wonschik</t>
         </is>
       </c>
     </row>
     <row r="152" ht="12.75" customHeight="1" s="17">
       <c r="A152" t="inlineStr">
         <is>
-          <t>sigridunterstab</t>
+          <t>anturomeronunes</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Sigrid</t>
+          <t>Antu</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Unterstab</t>
+          <t>Romero Nunes</t>
         </is>
       </c>
     </row>
     <row r="153" ht="12.75" customHeight="1" s="17">
       <c r="A153" t="inlineStr">
         <is>
-          <t>siegfriedboehm</t>
+          <t>nilsbernstein</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Siegfried</t>
+          <t>Nils</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Boehm</t>
+          <t>Bernstein</t>
         </is>
       </c>
     </row>
     <row r="154" ht="12.75" customHeight="1" s="17">
       <c r="A154" t="inlineStr">
         <is>
-          <t>filippofonio</t>
+          <t>charlottelerchner</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Filippo</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Fonio</t>
+          <t>Lerchner</t>
         </is>
       </c>
     </row>
     <row r="155" ht="12.75" customHeight="1" s="17">
       <c r="A155" t="inlineStr">
         <is>
-          <t>genevievegenicot</t>
+          <t>stefaniebeckmann</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Geneviève</t>
+          <t>Stefanie</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Genicot</t>
+          <t>Beckmann</t>
         </is>
       </c>
     </row>
     <row r="156" ht="12.75" customHeight="1" s="17">
       <c r="A156" t="inlineStr">
         <is>
-          <t>renatebreitig</t>
+          <t>gerlindekempendorffhoene</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Renate</t>
+          <t>Gerlinde</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Breitig</t>
+          <t>Kempendorff-Hoene</t>
         </is>
       </c>
     </row>
     <row r="157" ht="12.75" customHeight="1" s="17">
       <c r="A157" t="inlineStr">
         <is>
-          <t>christianegunther</t>
+          <t>stefaniejohn</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Christiane</t>
+          <t>Stefanie</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Günther</t>
+          <t>John</t>
         </is>
       </c>
     </row>
     <row r="158" ht="12.75" customHeight="1" s="17">
       <c r="A158" t="inlineStr">
         <is>
-          <t>racheldarby</t>
+          <t>hughleonard</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Rachel</t>
+          <t>Hugh</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Darby</t>
+          <t>Leonard</t>
         </is>
       </c>
     </row>
     <row r="159" ht="12.75" customHeight="1" s="17">
       <c r="A159" t="inlineStr">
         <is>
-          <t>wolfgangsting</t>
+          <t>wonkim</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Wolfgang</t>
+          <t>Won</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Sting</t>
+          <t>Kim</t>
         </is>
       </c>
     </row>
     <row r="160" ht="12.75" customHeight="1" s="17">
       <c r="A160" t="inlineStr">
         <is>
-          <t>juliakinze</t>
+          <t>alkistiskondoyianni</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Julia</t>
+          <t>Alkistis</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Kinze</t>
+          <t>Kondoyianni</t>
         </is>
       </c>
     </row>
     <row r="161" ht="12.75" customHeight="1" s="17">
       <c r="A161" t="inlineStr">
         <is>
-          <t>romidomkowsky</t>
+          <t>antonislenakakis</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Romi</t>
+          <t>Antonis</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Domkowsky</t>
+          <t>Lenakakis</t>
         </is>
       </c>
     </row>
     <row r="162" ht="12.75" customHeight="1" s="17">
       <c r="A162" t="inlineStr">
         <is>
-          <t>michafleiner</t>
+          <t>nikostsiotsos</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Micha</t>
+          <t>Nikos</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Fleiner</t>
+          <t>Tsiotsos</t>
         </is>
       </c>
     </row>
     <row r="163" ht="12.75" customHeight="1" s="17">
       <c r="A163" t="inlineStr">
         <is>
-          <t>nicolettamarinimaio</t>
+          <t>logamurthieathiemoolam</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Nicoletta</t>
+          <t>Logamurthie</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Marini-Maio</t>
+          <t>Athiemoolam</t>
         </is>
       </c>
     </row>
     <row r="164" ht="12.75" customHeight="1" s="17">
       <c r="A164" t="inlineStr">
         <is>
-          <t>andreapennacchi</t>
+          <t>lawarnsirisrimangkorn</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Lawarn</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Pennacchi</t>
+          <t>Sirisrimangkorn</t>
         </is>
       </c>
     </row>
     <row r="165" ht="12.75" customHeight="1" s="17">
       <c r="A165" t="inlineStr">
         <is>
-          <t>lornacarson</t>
+          <t>jitpanatsuwanthep</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Lorna</t>
+          <t>Jitpanat</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Carson</t>
+          <t>Suwanthep</t>
         </is>
       </c>
     </row>
     <row r="166" ht="12.75" customHeight="1" s="17">
       <c r="A166" t="inlineStr">
         <is>
-          <t>ivanlombardi</t>
+          <t>stefankriechbaumer</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Stefan</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Lombardi</t>
+          <t>Kriechbaumer</t>
         </is>
       </c>
     </row>
     <row r="167" ht="12.75" customHeight="1" s="17">
       <c r="A167" t="inlineStr">
         <is>
-          <t>claudiobendazzoli</t>
+          <t>maxpeterammann</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Claudio</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Bendazzoli</t>
+          <t>Peter Ammann</t>
         </is>
       </c>
     </row>
     <row r="168" ht="12.75" customHeight="1" s="17">
       <c r="A168" t="inlineStr">
         <is>
-          <t>yvonnegrimaldi</t>
+          <t>anabeaven</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Yvonne</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Grimaldi</t>
+          <t>Beaven</t>
         </is>
       </c>
     </row>
     <row r="169" ht="12.75" customHeight="1" s="17">
       <c r="A169" t="inlineStr">
         <is>
-          <t>gabriellacaponidoherty</t>
+          <t>inmaalvarez</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Gabriella</t>
+          <t>Inma</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Caponi-Doherty</t>
+          <t>Alvarez</t>
         </is>
       </c>
     </row>
     <row r="170" ht="12.75" customHeight="1" s="17">
       <c r="A170" t="inlineStr">
         <is>
-          <t>jensulrichdavids</t>
+          <t>jonathansharp</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Jens-Ulrich</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Davids</t>
+          <t>Sharp</t>
         </is>
       </c>
     </row>
     <row r="171" ht="12.75" customHeight="1" s="17">
       <c r="A171" t="inlineStr">
         <is>
-          <t>karelzdarek</t>
+          <t>clairekennedy</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Karel</t>
+          <t>Claire</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Zdarek</t>
+          <t>Kennedy</t>
         </is>
       </c>
     </row>
     <row r="172" ht="12.75" customHeight="1" s="17">
       <c r="A172" t="inlineStr">
         <is>
-          <t>theresabirnbaum</t>
+          <t>alexanderriedmuller</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Theresa</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Birnbaum</t>
+          <t>Riedmüller</t>
         </is>
       </c>
     </row>
     <row r="173" ht="12.75" customHeight="1" s="17">
       <c r="A173" t="inlineStr">
         <is>
-          <t>michaelasambanis</t>
+          <t>hanneseitz</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Michaela</t>
+          <t>Hanne</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Sambanis</t>
+          <t>Seitz</t>
         </is>
       </c>
     </row>
     <row r="174" ht="12.75" customHeight="1" s="17">
       <c r="A174" t="inlineStr">
         <is>
-          <t>delilbaran</t>
+          <t>morgankoerner</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Delil</t>
+          <t>Morgan</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Baran</t>
+          <t>Koerner</t>
         </is>
       </c>
     </row>
     <row r="175" ht="12.75" customHeight="1" s="17">
       <c r="A175" t="inlineStr">
         <is>
-          <t>kimonbeltrop</t>
+          <t>deborahnewton</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Kimon</t>
+          <t>Deborah</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Beltrop</t>
+          <t>Newton</t>
         </is>
       </c>
     </row>
     <row r="176" ht="12.75" customHeight="1" s="17">
       <c r="A176" t="inlineStr">
         <is>
-          <t>lisagrabert</t>
+          <t>annegretthiem</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Lisa</t>
+          <t>Annegret</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Grabert</t>
+          <t>Thiem</t>
         </is>
       </c>
     </row>
     <row r="177" ht="12.75" customHeight="1" s="17">
       <c r="A177" t="inlineStr">
         <is>
-          <t>janinaknorrdadfar</t>
+          <t>ankestoverblahak</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Janina</t>
+          <t>Anke</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Knorr-Dadfar</t>
+          <t>Stöver-Blahak</t>
         </is>
       </c>
     </row>
     <row r="178" ht="12.75" customHeight="1" s="17">
       <c r="A178" t="inlineStr">
         <is>
-          <t>josephinmarz</t>
+          <t>alexandrahensel</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Josephin</t>
+          <t>Alexandra</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>März</t>
+          <t>Hensel</t>
         </is>
       </c>
     </row>
     <row r="179" ht="12.75" customHeight="1" s="17">
       <c r="A179" t="inlineStr">
         <is>
-          <t>andreaschneider</t>
+          <t>ninakulovics</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Nina</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Schneider</t>
+          <t>Kulovics</t>
         </is>
       </c>
     </row>
     <row r="180" ht="12.75" customHeight="1" s="17">
       <c r="A180" t="inlineStr">
         <is>
-          <t>franksplitt</t>
+          <t>kerstinterler</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Kerstin</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Splitt</t>
+          <t>Terler</t>
         </is>
       </c>
     </row>
     <row r="181" ht="12.75" customHeight="1" s="17">
       <c r="A181" t="inlineStr">
         <is>
-          <t>katharinawonschik</t>
+          <t>leticiagarciabrea</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Katharina</t>
+          <t>Leticia</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Wonschik</t>
+          <t>García Brea</t>
         </is>
       </c>
     </row>
     <row r="182" ht="12.75" customHeight="1" s="17">
       <c r="A182" t="inlineStr">
         <is>
-          <t>nilsbernstein</t>
+          <t>isobelniriain</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Nils</t>
+          <t>Isobel</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Bernstein</t>
+          <t>Ní Riain</t>
         </is>
       </c>
     </row>
     <row r="183" ht="12.75" customHeight="1" s="17">
       <c r="A183" t="inlineStr">
         <is>
-          <t>charlottelerchner</t>
+          <t>nataliiadzhyma</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Nataliia</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Lerchner</t>
+          <t>Dzhyma</t>
         </is>
       </c>
     </row>
     <row r="184" ht="12.75" customHeight="1" s="17">
       <c r="A184" t="inlineStr">
         <is>
-          <t>gerlindekempendorffhoene</t>
+          <t>johncrutchfield</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Gerlinde</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Kempendorff-Hoene</t>
+          <t>Crutchfield</t>
         </is>
       </c>
     </row>
     <row r="185" ht="12.75" customHeight="1" s="17">
       <c r="A185" t="inlineStr">
         <is>
-          <t>stefaniejohn</t>
+          <t>bokjacho</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Stefanie</t>
+          <t>Bokja</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Cho</t>
         </is>
       </c>
     </row>
     <row r="186" ht="12.75" customHeight="1" s="17">
       <c r="A186" t="inlineStr">
         <is>
-          <t>hughleonard</t>
+          <t>martinaturecek</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Hugh</t>
+          <t>Martina</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Leonard</t>
+          <t>Turecek</t>
         </is>
       </c>
     </row>
     <row r="187" ht="12.75" customHeight="1" s="17">
       <c r="A187" t="inlineStr">
         <is>
-          <t>wonkim</t>
+          <t>philippbotes</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Won</t>
+          <t>Philipp</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Botes</t>
         </is>
       </c>
     </row>
     <row r="188" ht="12.75" customHeight="1" s="17">
       <c r="A188" t="inlineStr">
         <is>
-          <t>alkistiskondoyianni</t>
+          <t>danielberghoff</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Alkistis</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Kondoyianni</t>
+          <t>Berghoff</t>
         </is>
       </c>
     </row>
     <row r="189" ht="12.75" customHeight="1" s="17">
       <c r="A189" t="inlineStr">
         <is>
-          <t>antonislenakakis</t>
+          <t>peadardonohoe</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Antonis</t>
+          <t>Peadar</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Lenakakis</t>
+          <t>Donohoe</t>
         </is>
       </c>
     </row>
     <row r="190" ht="12.75" customHeight="1" s="17">
       <c r="A190" t="inlineStr">
         <is>
-          <t>nikostsiotsos</t>
+          <t>kristinwestphal</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Nikos</t>
+          <t>Kristin</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Tsiotsos</t>
+          <t>Westphal</t>
         </is>
       </c>
     </row>
     <row r="191" ht="12.75" customHeight="1" s="17">
       <c r="A191" t="inlineStr">
         <is>
-          <t>logamurthieathiemoolam</t>
+          <t>sabinedengscherz</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Logamurthie</t>
+          <t>Sabine</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Athiemoolam</t>
+          <t>Dengscherz</t>
         </is>
       </c>
     </row>
     <row r="192" ht="12.75" customHeight="1" s="17">
       <c r="A192" t="inlineStr">
         <is>
-          <t>lawarnsirisrimangkorn</t>
+          <t>sophiecharlotterummel</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Lawarn</t>
+          <t>Sophie</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Sirisrimangkorn</t>
+          <t>Charlotte Rummel</t>
         </is>
       </c>
     </row>
     <row r="193" ht="12.75" customHeight="1" s="17">
       <c r="A193" t="inlineStr">
         <is>
-          <t>jitpanatsuwanthep</t>
+          <t>angelikailg</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Jitpanat</t>
+          <t>Angelika</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Suwanthep</t>
+          <t>Ilg</t>
         </is>
       </c>
     </row>
     <row r="194" ht="12.75" customHeight="1" s="17">
       <c r="A194" t="inlineStr">
         <is>
-          <t>stefankriechbaumer</t>
+          <t>sabinekutzelmann</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Stefan</t>
+          <t>Sabine</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Kriechbaumer</t>
+          <t>Kutzelmann</t>
         </is>
       </c>
     </row>
     <row r="195" ht="12.75" customHeight="1" s="17">
       <c r="A195" t="inlineStr">
         <is>
-          <t>anabeaven</t>
+          <t>utemassler</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Ute</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Beaven</t>
+          <t>Massler</t>
         </is>
       </c>
     </row>
     <row r="196" ht="12.75" customHeight="1" s="17">
       <c r="A196" t="inlineStr">
         <is>
-          <t>inmaalvarez</t>
+          <t>klauspeter</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Inma</t>
+          <t>Klaus</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Alvarez</t>
+          <t>Peter</t>
         </is>
       </c>
     </row>
     <row r="197" ht="12.75" customHeight="1" s="17">
       <c r="A197" t="inlineStr">
         <is>
-          <t>clairekennedy</t>
+          <t>kerstintheinert</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Claire</t>
+          <t>Kerstin</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Kennedy</t>
+          <t>Theinert</t>
         </is>
       </c>
     </row>
     <row r="198" ht="12.75" customHeight="1" s="17">
       <c r="A198" t="inlineStr">
         <is>
-          <t>alexanderriedmuller</t>
+          <t>michaelareinhardt</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Michaela</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Riedmüller</t>
+          <t>Reinhardt</t>
         </is>
       </c>
     </row>
     <row r="199" ht="12.75" customHeight="1" s="17">
       <c r="A199" t="inlineStr">
         <is>
-          <t>morgankoerner</t>
+          <t>umbertocapra</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Morgan</t>
+          <t>Umberto</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Koerner</t>
+          <t>Capra</t>
         </is>
       </c>
     </row>
     <row r="200" ht="12.75" customHeight="1" s="17">
       <c r="A200" t="inlineStr">
         <is>
-          <t>deborahnewton</t>
+          <t>abigailpaul</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Deborah</t>
+          <t>Abigail</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Newton</t>
+          <t>Paul</t>
         </is>
       </c>
     </row>
     <row r="201" ht="12.75" customHeight="1" s="17">
       <c r="A201" t="inlineStr">
         <is>
-          <t>annegretthiem</t>
+          <t>annesmith</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Annegret</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Thiem</t>
+          <t>Smith</t>
         </is>
       </c>
     </row>
     <row r="202" ht="12.75" customHeight="1" s="17">
       <c r="A202" t="inlineStr">
         <is>
-          <t>ankestoverblahak</t>
+          <t>konstantinakalogirou</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Anke</t>
+          <t>Konstantina</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Stöver-Blahak</t>
+          <t>Kalogirou</t>
         </is>
       </c>
     </row>
     <row r="203" ht="12.75" customHeight="1" s="17">
       <c r="A203" t="inlineStr">
         <is>
-          <t>alexandrahensel</t>
+          <t>robinreid</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Alexandra</t>
+          <t>Robin</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Hensel</t>
+          <t>Reid</t>
         </is>
       </c>
     </row>
     <row r="204" ht="12.75" customHeight="1" s="17">
       <c r="A204" t="inlineStr">
         <is>
-          <t>ninakulovics</t>
+          <t>alinevennemann</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Nina</t>
+          <t>Aline</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Kulovics</t>
+          <t>Vennemann</t>
         </is>
       </c>
     </row>
     <row r="205" ht="12.75" customHeight="1" s="17">
       <c r="A205" t="inlineStr">
         <is>
-          <t>kerstinterler</t>
+          <t>simoneheinkhatib</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Kerstin</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Terler</t>
+          <t>Hein-Khatib</t>
         </is>
       </c>
     </row>
     <row r="206" ht="12.75" customHeight="1" s="17">
       <c r="A206" t="inlineStr">
         <is>
-          <t>nataliiadzhyma</t>
+          <t>marvinschildmeier</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Nataliia</t>
+          <t>Marvin</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Dzhyma</t>
+          <t>Schildmeier</t>
         </is>
       </c>
     </row>
     <row r="207" ht="12.75" customHeight="1" s="17">
       <c r="A207" t="inlineStr">
         <is>
-          <t>annesmith</t>
+          <t>liligrun</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Grün</t>
         </is>
       </c>
     </row>
     <row r="208" ht="12.75" customHeight="1" s="17">
       <c r="A208" t="inlineStr">
         <is>
-          <t>konstantinakalogirou</t>
+          <t>richardbale</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Konstantina</t>
+          <t>Richard</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Kalogirou</t>
+          <t>Bale</t>
         </is>
       </c>
     </row>
     <row r="209" ht="12.75" customHeight="1" s="17">
       <c r="A209" t="inlineStr">
         <is>
-          <t>robinreid</t>
+          <t>matthewmichaud</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Robin</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Reid</t>
+          <t>Michaud</t>
         </is>
       </c>
     </row>
     <row r="210" ht="12.75" customHeight="1" s="17">
       <c r="A210" t="inlineStr">
         <is>
-          <t>alinevennemann</t>
+          <t>toddhooper</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Aline</t>
+          <t>Todd</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Vennemann</t>
+          <t>Hooper</t>
         </is>
       </c>
     </row>
     <row r="211" ht="12.75" customHeight="1" s="17">
       <c r="A211" t="inlineStr">
         <is>
-          <t>simoneheinkhatib</t>
+          <t>albabordetas</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Alba</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Hein-Khatib</t>
+          <t>Bordetas</t>
         </is>
       </c>
     </row>
     <row r="212" ht="12.75" customHeight="1" s="17">
       <c r="A212" t="inlineStr">
         <is>
-          <t>marvinschildmeier</t>
+          <t>yasukoshiozawa</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Marvin</t>
+          <t>Yasuko</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Schildmeier</t>
+          <t>Shiozawa</t>
         </is>
       </c>
     </row>
     <row r="213" ht="12.75" customHeight="1" s="17">
       <c r="A213" t="inlineStr">
         <is>
-          <t>liligrun</t>
+          <t>mihomoody</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Miho</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Grün</t>
+          <t>Moody</t>
         </is>
       </c>
     </row>
     <row r="214" ht="12.75" customHeight="1" s="17">
       <c r="A214" t="inlineStr">
         <is>
-          <t>richardbale</t>
+          <t>benjaminswakopf</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Benjamin</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Bale</t>
+          <t>Swakopf</t>
         </is>
       </c>
     </row>
     <row r="215" ht="12.75" customHeight="1" s="17">
       <c r="A215" t="inlineStr">
         <is>
-          <t>matthewmichaud</t>
+          <t>dagmarhoffererbrunthaler</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Dagmar</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Michaud</t>
+          <t>Höfferer-Brunthaler</t>
         </is>
       </c>
     </row>
     <row r="216" ht="12.75" customHeight="1" s="17">
       <c r="A216" t="inlineStr">
         <is>
-          <t>toddhooper</t>
+          <t>amirhosseinesmkhani</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Todd</t>
+          <t>Amir</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Hooper</t>
+          <t>Hossein Esmkhani</t>
         </is>
       </c>
     </row>
     <row r="217" ht="12.75" customHeight="1" s="17">
       <c r="A217" t="inlineStr">
         <is>
-          <t>albabordetas</t>
+          <t>sandrineeschenauer</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Alba</t>
+          <t>Sandrine</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Bordetas</t>
+          <t>Eschenauer</t>
         </is>
       </c>
     </row>
     <row r="218" ht="12.75" customHeight="1" s="17">
       <c r="A218" t="inlineStr">
         <is>
-          <t>yasukoshiozawa</t>
+          <t>ninahasenzagl</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Yasuko</t>
+          <t>Nina</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Shiozawa</t>
+          <t>Hasenzagl</t>
         </is>
       </c>
     </row>
     <row r="219" ht="12.75" customHeight="1" s="17">
       <c r="A219" t="inlineStr">
         <is>
-          <t>mihomoody</t>
+          <t>annesteiner</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Miho</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Moody</t>
+          <t>Steiner</t>
         </is>
       </c>
     </row>
     <row r="220" ht="12.75" customHeight="1" s="17">
       <c r="A220" t="inlineStr">
         <is>
-          <t>benjaminswakopf</t>
+          <t>lanesorensen</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Lane</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Swakopf</t>
+          <t>Sorensen</t>
         </is>
       </c>
     </row>
     <row r="221" ht="12.75" customHeight="1" s="17">
       <c r="A221" t="inlineStr">
         <is>
-          <t>dagmarhoffererbrunthaler</t>
+          <t>patriciaklich</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Dagmar</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Höfferer-Brunthaler</t>
+          <t>Klich</t>
         </is>
       </c>
     </row>
     <row r="222" ht="12.75" customHeight="1" s="17">
       <c r="A222" t="inlineStr">
         <is>
-          <t>sandrineeschenauer</t>
+          <t>maciekklich</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Sandrine</t>
+          <t>Maciek</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Eschenauer</t>
+          <t>Klich</t>
         </is>
       </c>
     </row>
     <row r="223" ht="12.75" customHeight="1" s="17">
       <c r="A223" t="inlineStr">
         <is>
-          <t>ninahasenzagl</t>
+          <t>kathleenrosemcgovern</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Nina</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Hasenzagl</t>
+          <t>Rose McGovern</t>
         </is>
       </c>
     </row>
     <row r="224" ht="12.75" customHeight="1" s="17">
       <c r="A224" t="inlineStr">
         <is>
-          <t>annesteiner</t>
+          <t>monaeikelpohen</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Mona</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Steiner</t>
+          <t>Eikel-Pohen</t>
         </is>
       </c>
     </row>
     <row r="225" ht="12.75" customHeight="1" s="17">
       <c r="A225" t="inlineStr">
         <is>
-          <t>lanesorensen</t>
+          <t>leecampbell</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Lane</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Sorensen</t>
+          <t>Campbell</t>
         </is>
       </c>
     </row>
     <row r="226" ht="12.75" customHeight="1" s="17">
       <c r="A226" t="inlineStr">
         <is>
-          <t>patriciaklich</t>
+          <t>catherinevanhalsema</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Catherine</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Klich</t>
+          <t>Van Halsema</t>
         </is>
       </c>
     </row>
     <row r="227" ht="12.75" customHeight="1" s="17">
       <c r="A227" t="inlineStr">
         <is>
-          <t>maciekklich</t>
+          <t>ciarandawson</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Maciek</t>
+          <t>Ciarán</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Klich</t>
+          <t>Dawson</t>
         </is>
       </c>
     </row>
     <row r="228" ht="12.75" customHeight="1" s="17">
       <c r="A228" t="inlineStr">
         <is>
-          <t>monaeikelpohen</t>
+          <t>marianmccarthy</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Mona</t>
+          <t>Marian</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Eikel-Pohen</t>
+          <t>McCarthy</t>
         </is>
       </c>
     </row>
     <row r="229" ht="12.75" customHeight="1" s="17">
       <c r="A229" t="inlineStr">
         <is>
-          <t>leecampbell</t>
+          <t>tomklimant</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Campbell</t>
+          <t>Klimant</t>
         </is>
       </c>
     </row>
     <row r="230" ht="12.75" customHeight="1" s="17">
       <c r="A230" t="inlineStr">
         <is>
-          <t>ciarandawson</t>
+          <t>uschilinehan</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Ciarán</t>
+          <t>Uschi</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Dawson</t>
+          <t>Linehan</t>
         </is>
       </c>
     </row>
     <row r="231" ht="12.75" customHeight="1" s="17">
       <c r="A231" t="inlineStr">
         <is>
-          <t>marianmccarthy</t>
+          <t>gustavejweltsek</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Marian</t>
+          <t>Gustave</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>McCarthy</t>
+          <t>J. Weltsek</t>
         </is>
       </c>
     </row>
     <row r="232" ht="12.75" customHeight="1" s="17">
       <c r="A232" t="inlineStr">
         <is>
-          <t>tomklimant</t>
+          <t>petrabosenius</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Petra</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Klimant</t>
+          <t>Bosenius</t>
         </is>
       </c>
     </row>
     <row r="233" ht="12.75" customHeight="1" s="17">
       <c r="A233" t="inlineStr">
         <is>
-          <t>uschilinehan</t>
+          <t>susannehorstmann</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Uschi</t>
+          <t>Susanne</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Linehan</t>
+          <t>Horstmann</t>
         </is>
       </c>
     </row>
     <row r="234" ht="12.75" customHeight="1" s="17">
       <c r="A234" t="inlineStr">
         <is>
-          <t>petrabosenius</t>
+          <t>serafinamorrin</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Petra</t>
+          <t>Serafina</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Bosenius</t>
+          <t>Morrin</t>
         </is>
       </c>
     </row>
     <row r="235" ht="12.75" customHeight="1" s="17">
       <c r="A235" t="inlineStr">
         <is>
-          <t>susannehorstmann</t>
+          <t>francescobonelli</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Susanne</t>
+          <t>Francesco</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Horstmann</t>
+          <t>Bonelli</t>
         </is>
       </c>
     </row>
     <row r="236" ht="12.75" customHeight="1" s="17">
       <c r="A236" t="inlineStr">
         <is>
-          <t>serafinamorrin</t>
+          <t>stefanblutner</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Serafina</t>
+          <t>Stefan</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Morrin</t>
+          <t>Blutner</t>
         </is>
       </c>
     </row>
     <row r="237" ht="12.75" customHeight="1" s="17">
       <c r="A237" t="inlineStr">
         <is>
-          <t>francescobonelli</t>
+          <t>andrebastian</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Francesco</t>
+          <t>André</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Bonelli</t>
+          <t>Bastian</t>
         </is>
       </c>
     </row>
     <row r="238" ht="12.75" customHeight="1" s="17">
       <c r="A238" t="inlineStr">
         <is>
-          <t>stefanblutner</t>
+          <t>melaniebloom</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Stefan</t>
+          <t>Melanie</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Blutner</t>
+          <t>Bloom</t>
         </is>
       </c>
     </row>
     <row r="239" ht="12.75" customHeight="1" s="17">
       <c r="A239" t="inlineStr">
         <is>
-          <t>andrebastian</t>
+          <t>perihankorkut</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>André</t>
+          <t>Perihan</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Bastian</t>
+          <t>Korkut</t>
         </is>
       </c>
     </row>
     <row r="240" ht="12.75" customHeight="1" s="17">
       <c r="A240" t="inlineStr">
         <is>
-          <t>melaniebloom</t>
+          <t>michaelklegutke</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Bloom</t>
+          <t>K. Legutke</t>
         </is>
       </c>
     </row>
     <row r="241" ht="12.75" customHeight="1" s="17">
       <c r="A241" t="inlineStr">
         <is>
-          <t>perihankorkut</t>
+          <t>tinwegel</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Perihan</t>
+          <t>Tin</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Korkut</t>
+          <t>Wegel</t>
         </is>
       </c>
     </row>
     <row r="242" ht="12.75" customHeight="1" s="17">
       <c r="A242" t="inlineStr">
         <is>
-          <t>tinwegel</t>
+          <t>hughwalpole</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Tin</t>
+          <t>Hugh</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Wegel</t>
+          <t>Walpole</t>
         </is>
       </c>
     </row>
     <row r="243" ht="12.75" customHeight="1" s="17">
       <c r="A243" t="inlineStr">
         <is>
-          <t>hughwalpole</t>
+          <t>erinnoelliste</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Hugh</t>
+          <t>Erin</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Walpole</t>
+          <t>Noelliste</t>
         </is>
       </c>
     </row>
     <row r="244" ht="12.75" customHeight="1" s="17">
       <c r="A244" t="inlineStr">
         <is>
-          <t>erinnoelliste</t>
+          <t>josephnoelliste</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -15295,17 +15307,17 @@
     <row r="245" ht="12.75" customHeight="1" s="17">
       <c r="A245" t="inlineStr">
         <is>
-          <t>josephnoelliste</t>
+          <t>konstantinosprokopiostrimmis</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Konstantinos</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Noelliste</t>
+          <t>Prokopios Trimmis</t>
         </is>
       </c>
     </row>
@@ -16012,6 +16024,186 @@
     <row r="818" ht="12.75" customHeight="1" s="17"/>
     <row r="819" ht="12.75" customHeight="1" s="17"/>
     <row r="820" ht="12.75" customHeight="1" s="17"/>
+    <row r="821" ht="12.75" customHeight="1" s="17"/>
+    <row r="822" ht="12.75" customHeight="1" s="17"/>
+    <row r="823" ht="12.75" customHeight="1" s="17"/>
+    <row r="824" ht="12.75" customHeight="1" s="17"/>
+    <row r="825" ht="12.75" customHeight="1" s="17"/>
+    <row r="826" ht="12.75" customHeight="1" s="17"/>
+    <row r="827" ht="12.75" customHeight="1" s="17"/>
+    <row r="828" ht="12.75" customHeight="1" s="17"/>
+    <row r="829" ht="12.75" customHeight="1" s="17"/>
+    <row r="830" ht="12.75" customHeight="1" s="17"/>
+    <row r="831" ht="12.75" customHeight="1" s="17"/>
+    <row r="832" ht="12.75" customHeight="1" s="17"/>
+    <row r="833" ht="12.75" customHeight="1" s="17"/>
+    <row r="834" ht="12.75" customHeight="1" s="17"/>
+    <row r="835" ht="12.75" customHeight="1" s="17"/>
+    <row r="836" ht="12.75" customHeight="1" s="17"/>
+    <row r="837" ht="12.75" customHeight="1" s="17"/>
+    <row r="838" ht="12.75" customHeight="1" s="17"/>
+    <row r="839" ht="12.75" customHeight="1" s="17"/>
+    <row r="840" ht="12.75" customHeight="1" s="17"/>
+    <row r="841" ht="12.75" customHeight="1" s="17"/>
+    <row r="842" ht="12.75" customHeight="1" s="17"/>
+    <row r="843" ht="12.75" customHeight="1" s="17"/>
+    <row r="844" ht="12.75" customHeight="1" s="17"/>
+    <row r="845" ht="12.75" customHeight="1" s="17"/>
+    <row r="846" ht="12.75" customHeight="1" s="17"/>
+    <row r="847" ht="12.75" customHeight="1" s="17"/>
+    <row r="848" ht="12.75" customHeight="1" s="17"/>
+    <row r="849" ht="12.75" customHeight="1" s="17"/>
+    <row r="850" ht="12.75" customHeight="1" s="17"/>
+    <row r="851" ht="12.75" customHeight="1" s="17"/>
+    <row r="852" ht="12.75" customHeight="1" s="17"/>
+    <row r="853" ht="12.75" customHeight="1" s="17"/>
+    <row r="854" ht="12.75" customHeight="1" s="17"/>
+    <row r="855" ht="12.75" customHeight="1" s="17"/>
+    <row r="856" ht="12.75" customHeight="1" s="17"/>
+    <row r="857" ht="12.75" customHeight="1" s="17"/>
+    <row r="858" ht="12.75" customHeight="1" s="17"/>
+    <row r="859" ht="12.75" customHeight="1" s="17"/>
+    <row r="860" ht="12.75" customHeight="1" s="17"/>
+    <row r="861" ht="12.75" customHeight="1" s="17"/>
+    <row r="862" ht="12.75" customHeight="1" s="17"/>
+    <row r="863" ht="12.75" customHeight="1" s="17"/>
+    <row r="864" ht="12.75" customHeight="1" s="17"/>
+    <row r="865" ht="12.75" customHeight="1" s="17"/>
+    <row r="866" ht="12.75" customHeight="1" s="17"/>
+    <row r="867" ht="12.75" customHeight="1" s="17"/>
+    <row r="868" ht="12.75" customHeight="1" s="17"/>
+    <row r="869" ht="12.75" customHeight="1" s="17"/>
+    <row r="870" ht="12.75" customHeight="1" s="17"/>
+    <row r="871" ht="12.75" customHeight="1" s="17"/>
+    <row r="872" ht="12.75" customHeight="1" s="17"/>
+    <row r="873" ht="12.75" customHeight="1" s="17"/>
+    <row r="874" ht="12.75" customHeight="1" s="17"/>
+    <row r="875" ht="12.75" customHeight="1" s="17"/>
+    <row r="876" ht="12.75" customHeight="1" s="17"/>
+    <row r="877" ht="12.75" customHeight="1" s="17"/>
+    <row r="878" ht="12.75" customHeight="1" s="17"/>
+    <row r="879" ht="12.75" customHeight="1" s="17"/>
+    <row r="880" ht="12.75" customHeight="1" s="17"/>
+    <row r="881" ht="12.75" customHeight="1" s="17"/>
+    <row r="882" ht="12.75" customHeight="1" s="17"/>
+    <row r="883" ht="12.75" customHeight="1" s="17"/>
+    <row r="884" ht="12.75" customHeight="1" s="17"/>
+    <row r="885" ht="12.75" customHeight="1" s="17"/>
+    <row r="886" ht="12.75" customHeight="1" s="17"/>
+    <row r="887" ht="12.75" customHeight="1" s="17"/>
+    <row r="888" ht="12.75" customHeight="1" s="17"/>
+    <row r="889" ht="12.75" customHeight="1" s="17"/>
+    <row r="890" ht="12.75" customHeight="1" s="17"/>
+    <row r="891" ht="12.75" customHeight="1" s="17"/>
+    <row r="892" ht="12.75" customHeight="1" s="17"/>
+    <row r="893" ht="12.75" customHeight="1" s="17"/>
+    <row r="894" ht="12.75" customHeight="1" s="17"/>
+    <row r="895" ht="12.75" customHeight="1" s="17"/>
+    <row r="896" ht="12.75" customHeight="1" s="17"/>
+    <row r="897" ht="12.75" customHeight="1" s="17"/>
+    <row r="898" ht="12.75" customHeight="1" s="17"/>
+    <row r="899" ht="12.75" customHeight="1" s="17"/>
+    <row r="900" ht="12.75" customHeight="1" s="17"/>
+    <row r="901" ht="12.75" customHeight="1" s="17"/>
+    <row r="902" ht="12.75" customHeight="1" s="17"/>
+    <row r="903" ht="12.75" customHeight="1" s="17"/>
+    <row r="904" ht="12.75" customHeight="1" s="17"/>
+    <row r="905" ht="12.75" customHeight="1" s="17"/>
+    <row r="906" ht="12.75" customHeight="1" s="17"/>
+    <row r="907" ht="12.75" customHeight="1" s="17"/>
+    <row r="908" ht="12.75" customHeight="1" s="17"/>
+    <row r="909" ht="12.75" customHeight="1" s="17"/>
+    <row r="910" ht="12.75" customHeight="1" s="17"/>
+    <row r="911" ht="12.75" customHeight="1" s="17"/>
+    <row r="912" ht="12.75" customHeight="1" s="17"/>
+    <row r="913" ht="12.75" customHeight="1" s="17"/>
+    <row r="914" ht="12.75" customHeight="1" s="17"/>
+    <row r="915" ht="12.75" customHeight="1" s="17"/>
+    <row r="916" ht="12.75" customHeight="1" s="17"/>
+    <row r="917" ht="12.75" customHeight="1" s="17"/>
+    <row r="918" ht="12.75" customHeight="1" s="17"/>
+    <row r="919" ht="12.75" customHeight="1" s="17"/>
+    <row r="920" ht="12.75" customHeight="1" s="17"/>
+    <row r="921" ht="12.75" customHeight="1" s="17"/>
+    <row r="922" ht="12.75" customHeight="1" s="17"/>
+    <row r="923" ht="12.75" customHeight="1" s="17"/>
+    <row r="924" ht="12.75" customHeight="1" s="17"/>
+    <row r="925" ht="12.75" customHeight="1" s="17"/>
+    <row r="926" ht="12.75" customHeight="1" s="17"/>
+    <row r="927" ht="12.75" customHeight="1" s="17"/>
+    <row r="928" ht="12.75" customHeight="1" s="17"/>
+    <row r="929" ht="12.75" customHeight="1" s="17"/>
+    <row r="930" ht="12.75" customHeight="1" s="17"/>
+    <row r="931" ht="12.75" customHeight="1" s="17"/>
+    <row r="932" ht="12.75" customHeight="1" s="17"/>
+    <row r="933" ht="12.75" customHeight="1" s="17"/>
+    <row r="934" ht="12.75" customHeight="1" s="17"/>
+    <row r="935" ht="12.75" customHeight="1" s="17"/>
+    <row r="936" ht="12.75" customHeight="1" s="17"/>
+    <row r="937" ht="12.75" customHeight="1" s="17"/>
+    <row r="938" ht="12.75" customHeight="1" s="17"/>
+    <row r="939" ht="12.75" customHeight="1" s="17"/>
+    <row r="940" ht="12.75" customHeight="1" s="17"/>
+    <row r="941" ht="12.75" customHeight="1" s="17"/>
+    <row r="942" ht="12.75" customHeight="1" s="17"/>
+    <row r="943" ht="12.75" customHeight="1" s="17"/>
+    <row r="944" ht="12.75" customHeight="1" s="17"/>
+    <row r="945" ht="12.75" customHeight="1" s="17"/>
+    <row r="946" ht="12.75" customHeight="1" s="17"/>
+    <row r="947" ht="12.75" customHeight="1" s="17"/>
+    <row r="948" ht="12.75" customHeight="1" s="17"/>
+    <row r="949" ht="12.75" customHeight="1" s="17"/>
+    <row r="950" ht="12.75" customHeight="1" s="17"/>
+    <row r="951" ht="12.75" customHeight="1" s="17"/>
+    <row r="952" ht="12.75" customHeight="1" s="17"/>
+    <row r="953" ht="12.75" customHeight="1" s="17"/>
+    <row r="954" ht="12.75" customHeight="1" s="17"/>
+    <row r="955" ht="12.75" customHeight="1" s="17"/>
+    <row r="956" ht="12.75" customHeight="1" s="17"/>
+    <row r="957" ht="12.75" customHeight="1" s="17"/>
+    <row r="958" ht="12.75" customHeight="1" s="17"/>
+    <row r="959" ht="12.75" customHeight="1" s="17"/>
+    <row r="960" ht="12.75" customHeight="1" s="17"/>
+    <row r="961" ht="12.75" customHeight="1" s="17"/>
+    <row r="962" ht="12.75" customHeight="1" s="17"/>
+    <row r="963" ht="12.75" customHeight="1" s="17"/>
+    <row r="964" ht="12.75" customHeight="1" s="17"/>
+    <row r="965" ht="12.75" customHeight="1" s="17"/>
+    <row r="966" ht="12.75" customHeight="1" s="17"/>
+    <row r="967" ht="12.75" customHeight="1" s="17"/>
+    <row r="968" ht="12.75" customHeight="1" s="17"/>
+    <row r="969" ht="12.75" customHeight="1" s="17"/>
+    <row r="970" ht="12.75" customHeight="1" s="17"/>
+    <row r="971" ht="12.75" customHeight="1" s="17"/>
+    <row r="972" ht="12.75" customHeight="1" s="17"/>
+    <row r="973" ht="12.75" customHeight="1" s="17"/>
+    <row r="974" ht="12.75" customHeight="1" s="17"/>
+    <row r="975" ht="12.75" customHeight="1" s="17"/>
+    <row r="976" ht="12.75" customHeight="1" s="17"/>
+    <row r="977" ht="12.75" customHeight="1" s="17"/>
+    <row r="978" ht="12.75" customHeight="1" s="17"/>
+    <row r="979" ht="12.75" customHeight="1" s="17"/>
+    <row r="980" ht="12.75" customHeight="1" s="17"/>
+    <row r="981" ht="12.75" customHeight="1" s="17"/>
+    <row r="982" ht="12.75" customHeight="1" s="17"/>
+    <row r="983" ht="12.75" customHeight="1" s="17"/>
+    <row r="984" ht="12.75" customHeight="1" s="17"/>
+    <row r="985" ht="12.75" customHeight="1" s="17"/>
+    <row r="986" ht="12.75" customHeight="1" s="17"/>
+    <row r="987" ht="12.75" customHeight="1" s="17"/>
+    <row r="988" ht="12.75" customHeight="1" s="17"/>
+    <row r="989" ht="12.75" customHeight="1" s="17"/>
+    <row r="990" ht="12.75" customHeight="1" s="17"/>
+    <row r="991" ht="12.75" customHeight="1" s="17"/>
+    <row r="992" ht="12.75" customHeight="1" s="17"/>
+    <row r="993" ht="12.75" customHeight="1" s="17"/>
+    <row r="994" ht="12.75" customHeight="1" s="17"/>
+    <row r="995" ht="12.75" customHeight="1" s="17"/>
+    <row r="996" ht="12.75" customHeight="1" s="17"/>
+    <row r="997" ht="12.75" customHeight="1" s="17"/>
+    <row r="998" ht="12.75" customHeight="1" s="17"/>
+    <row r="999" ht="12.75" customHeight="1" s="17"/>
+    <row r="1000" ht="12.75" customHeight="1" s="17"/>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G2" r:id="rId1"/>
@@ -16080,21 +16272,21 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="25.265625" customWidth="1" style="17" min="1" max="1"/>
-    <col width="198.265625" customWidth="1" style="17" min="2" max="2"/>
-    <col width="31.1328125" customWidth="1" style="17" min="3" max="3"/>
-    <col width="8.265625" customWidth="1" style="17" min="4" max="4"/>
-    <col width="16.73046875" customWidth="1" style="17" min="5" max="5"/>
-    <col width="21.265625" customWidth="1" style="17" min="6" max="6"/>
-    <col width="8.86328125" customWidth="1" style="17" min="7" max="10"/>
+    <col width="25.28515625" customWidth="1" style="17" min="1" max="1"/>
+    <col width="198.28515625" customWidth="1" style="17" min="2" max="2"/>
+    <col width="31.140625" customWidth="1" style="17" min="3" max="3"/>
+    <col width="8.28515625" customWidth="1" style="17" min="4" max="4"/>
+    <col width="16.7109375" customWidth="1" style="17" min="5" max="5"/>
+    <col width="21.28515625" customWidth="1" style="17" min="6" max="6"/>
+    <col width="8.85546875" customWidth="1" style="17" min="7" max="10"/>
     <col width="11" customWidth="1" style="17" min="11" max="11"/>
-    <col width="8.86328125" customWidth="1" style="17" min="12" max="13"/>
-    <col width="27.1328125" customWidth="1" style="17" min="14" max="14"/>
-    <col width="29.86328125" customWidth="1" style="17" min="15" max="15"/>
-    <col width="19.265625" customWidth="1" style="17" min="16" max="16"/>
-    <col width="8.86328125" customWidth="1" style="17" min="17" max="26"/>
+    <col width="8.85546875" customWidth="1" style="17" min="12" max="13"/>
+    <col width="27.140625" customWidth="1" style="17" min="14" max="14"/>
+    <col width="29.85546875" customWidth="1" style="17" min="15" max="15"/>
+    <col width="19.28515625" customWidth="1" style="17" min="16" max="16"/>
+    <col width="8.85546875" customWidth="1" style="17" min="17" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12" customHeight="1" s="17">
@@ -16192,7 +16384,7 @@
       </c>
     </row>
     <row r="3" ht="12" customHeight="1" s="17">
-      <c r="B3" s="21" t="inlineStr">
+      <c r="B3" s="22" t="inlineStr">
         <is>
           <t>Emdin, Christopher (2013): Teach teachers how to create magic. Video file: https://www.ted.com/talks/christopher_emdin_teach_teachers_how_to_create_magic/discussion?utm_content=awesm-publisher&amp;utm_medium=on.ted.</t>
         </is>
@@ -16220,21 +16412,21 @@
       </c>
     </row>
     <row r="7" ht="12" customHeight="1" s="17">
-      <c r="B7" s="21" t="inlineStr">
+      <c r="B7" s="22" t="inlineStr">
         <is>
           <t>Robinson, Sir Ken (2011): Leading a learning revolution. Learning without frontiers. Video file: https://www.youtube.com/watch?v=-XTCSTW24Ss</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" s="17">
-      <c r="B8" s="21" t="inlineStr">
+      <c r="B8" s="22" t="inlineStr">
         <is>
           <t>Schewe, Manfred (2014): Four lively days…at the SCENARIO Forum International Conference 2014. Video file: https://www.youtube.com/watch?v=3dhpa6Yz5_M&amp;t=184s</t>
         </is>
       </c>
     </row>
     <row r="9" ht="12" customHeight="1" s="17">
-      <c r="B9" s="21" t="inlineStr">
+      <c r="B9" s="22" t="inlineStr">
         <is>
           <t>Terronez, Azul (2017): What makes a good teacher great? Video file: https://www.youtube.com/watch?v=vrU6YJle6Q4</t>
         </is>
@@ -16420,7 +16612,7 @@
       </c>
     </row>
     <row r="27" ht="12" customHeight="1" s="17">
-      <c r="B27" s="21" t="inlineStr">
+      <c r="B27" s="22" t="inlineStr">
         <is>
           <t>Mewald, Claudia (2015): Wonder: From novel to play: A project report. In: R&amp;E Source: Open Online Journal for Research and Education 2 http://journal.ph-noe.ac.at/index.php/resource/article/view/215/218 [last accessed July 15, 2019]</t>
         </is>
@@ -16428,7 +16620,7 @@
       <c r="C27" s="1" t="n"/>
     </row>
     <row r="28" ht="12" customHeight="1" s="17">
-      <c r="B28" s="21" t="inlineStr">
+      <c r="B28" s="22" t="inlineStr">
         <is>
           <t>Mewald, Claudia; Wallner, Sabine &amp; Weitz-Polydoros, Elisabeth (2016): All the world’s a stage: Educational drama &amp; Drama in education. In: R&amp;E Source: Open Online Journal for Research and Education https://journal.ph-noe.ac.at/index.php/resource/article/view/330 [last accessed July 15, 2019]</t>
         </is>
@@ -16807,7 +16999,7 @@
       </c>
     </row>
     <row r="72" ht="12" customHeight="1" s="17">
-      <c r="B72" s="21" t="inlineStr">
+      <c r="B72" s="22" t="inlineStr">
         <is>
           <t>Geneuss, Katrin (2019): „Die waren ja mittendrin!”. Ganzheitliches Lernen im Rollenspiel EduLARP. Grundlagen – Wirkungen – Einsatz im Deutschunterricht. In: Elektronische Hochschulschriften: Ludwig-Maximilians-Universität München [last accessed January 10, 2020]</t>
         </is>
@@ -16903,7 +17095,7 @@
       </c>
     </row>
     <row r="83" ht="12" customHeight="1" s="17">
-      <c r="B83" s="21" t="inlineStr">
+      <c r="B83" s="22" t="inlineStr">
         <is>
           <t>Neubauer, Alexander (2015): Liverollenspiel als Unterrichtsmethode. Potentiale und Risiken. https://1000atmosphaeren.at/2015/10/28/873/ [last accessed January 10, 2020]</t>
         </is>
@@ -16978,10 +17170,10 @@
           <t>Warwitz, Siegbert A. &amp; Rudolf, Anita (2016): Spielend ein anderer sein – Rollenspiele. In: Warwitz, Siegbert A. &amp; Rudolf, Anita (eds.): Vom Sinn des Spielens. Reflexionen und Spielideen. 4. Auflage. Baltmannsweiler: Schneider Hohengehren</t>
         </is>
       </c>
-      <c r="C91" s="21" t="n"/>
+      <c r="C91" s="22" t="n"/>
     </row>
     <row r="92" ht="12" customHeight="1" s="17">
-      <c r="B92" s="21" t="inlineStr">
+      <c r="B92" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Wirag, Andreas (2019): Experimentelle Studien zu Theaterarbeit und Persönlichkeitsentwicklung: Die aktuelle Befundlage. In: Scenario 13/2, 92-108 </t>
         </is>
@@ -17019,7 +17211,7 @@
       </c>
     </row>
     <row r="96" ht="12" customHeight="1" s="17">
-      <c r="B96" s="21" t="inlineStr">
+      <c r="B96" s="22" t="inlineStr">
         <is>
           <t>Dominguez Sapien, Natalia (2019): Macht kein (Psycho-)Drama draus! Dramapädagogik, Psychodrama, Psychodramaturgie: Versuch einer Begriffsklärung. In: Giebert, Stefanie &amp; Göksel, Eva (Hrsg.): Dramapädagogik-Tage 2018/Drama in Education Days 2018 – Conference Proceedings of the 4th Annual Conference on Performative Language Teaching and Learning, 23-31 https://dramapaedagogik.de/wp-content/uploads/Proceedings2018/final.pdf</t>
         </is>
@@ -17027,7 +17219,7 @@
       <c r="C96" s="1" t="n"/>
     </row>
     <row r="97" ht="12" customHeight="1" s="17">
-      <c r="B97" s="21" t="inlineStr">
+      <c r="B97" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Dufeu, Bernard (2013b): Das Doppeln in der Psychodramaturgie. In: Zeitschrift für Psychodrama und Soziometrie, Oktober, 173-187 </t>
         </is>
@@ -17046,7 +17238,7 @@
       </c>
     </row>
     <row r="99" ht="12" customHeight="1" s="17">
-      <c r="B99" s="21" t="inlineStr">
+      <c r="B99" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Dufeu, Bernard (2007): Die Bedeutung des Körpers in der Psychodramaturgie. In: Zeitschrift für Psychodrama und Soziometrie, März, 50-62 </t>
         </is>
@@ -17121,7 +17313,7 @@
       </c>
     </row>
     <row r="109" ht="12" customHeight="1" s="17">
-      <c r="B109" s="21" t="inlineStr">
+      <c r="B109" s="22" t="inlineStr">
         <is>
           <t>Dufeu, Bernard: Bibliographie über die PDL https://www.psychodramaturgie.org/de/publikationen/bibliografie</t>
         </is>
@@ -17142,7 +17334,7 @@
       </c>
     </row>
     <row r="112" ht="12" customHeight="1" s="17">
-      <c r="B112" s="21" t="inlineStr">
+      <c r="B112" s="22" t="inlineStr">
         <is>
           <t>Floridia, Aurora (2017) Die Psychodramaturgie Linguistique-Methode im Einzelsetting. In: Zeitschrift für Psychodrama und Soziometrie, Oktober, 319-333</t>
         </is>
@@ -17168,7 +17360,7 @@
       </c>
     </row>
     <row r="115" ht="12" customHeight="1" s="17">
-      <c r="B115" s="21" t="inlineStr">
+      <c r="B115" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Karnath, Hans-Otto &amp; Thier, Peter (2003): Neuropsychologie. Heidelberg: Springer Medizin Verlag </t>
         </is>
@@ -17255,14 +17447,14 @@
       </c>
     </row>
     <row r="126" ht="12" customHeight="1" s="17">
-      <c r="B126" s="21" t="inlineStr">
+      <c r="B126" s="22" t="inlineStr">
         <is>
           <t>Davis, Jeffrey (1990): Archetypal Puppets Spark Good Writing. In: College Teaching 38/2, 49-51, http://www.jstor.org/stable/27558392 [last accessed Jan 05, 2020]</t>
         </is>
       </c>
     </row>
     <row r="127" ht="12" customHeight="1" s="17">
-      <c r="B127" s="21" t="inlineStr">
+      <c r="B127" s="22" t="inlineStr">
         <is>
           <t>Egge, Debora, Marks, Lauren &amp; McEvers, Donna (1987): Puppets and Adolescents: A group guidance workshop approach. In: Elementary School Guidance &amp; Counseling 21/3 pp.183-192, http://www.jstor.org/stable/42869232 [last accessed Jan 05, 2020]</t>
         </is>
@@ -17276,21 +17468,21 @@
       </c>
     </row>
     <row r="129" ht="12" customHeight="1" s="17">
-      <c r="B129" s="21" t="inlineStr">
+      <c r="B129" s="22" t="inlineStr">
         <is>
           <t>Peck, Sharon &amp; Virkler, Aubre (2006): Reading in the Shadows: Extending Literacy Skills through Shadow-Puppet Theater. In: The Reading Teacher 59/8, 786-795, http://www.jstor.org/stable/20204419 [last accessed Jan 05, 2020]</t>
         </is>
       </c>
     </row>
     <row r="130" ht="12" customHeight="1" s="17">
-      <c r="B130" s="21" t="inlineStr">
+      <c r="B130" s="22" t="inlineStr">
         <is>
           <t>Willis, Judy (2007): The Neuroscience of Joyful Education. In: Educational Leadership 64: Engaging the Whole Child, online only (Summer 2007), http://www.ascd.org/publications/educational-leadership/summer07/vol64/num09/The-Neuroscience-of-Joyful-Education.aspx [last accessed Jan 05, 2020]</t>
         </is>
       </c>
     </row>
     <row r="131" ht="12" customHeight="1" s="17">
-      <c r="B131" s="21" t="inlineStr">
+      <c r="B131" s="22" t="inlineStr">
         <is>
           <t>van Rossum, Helene: Past Times – Activities and Resources to make history come alive, http://www.pasttimeshistory.com [last accessed Jan 05, 2020]</t>
         </is>
@@ -17323,7 +17515,7 @@
       </c>
     </row>
     <row r="135" ht="12" customHeight="1" s="17">
-      <c r="B135" s="21" t="inlineStr">
+      <c r="B135" s="22" t="inlineStr">
         <is>
           <t>Dunn, Julie &amp; Stinson, Madonna (2011): Not without the art!! The importance of teacher artistry when applying drama as pedagogy for additional language learning. In: Research in Drama Education 16/4, 617-633, https://doi.org/10.1080/13569783.2011.617110</t>
         </is>
@@ -17337,7 +17529,7 @@
       </c>
     </row>
     <row r="137" ht="12" customHeight="1" s="17">
-      <c r="B137" s="21" t="inlineStr">
+      <c r="B137" s="22" t="inlineStr">
         <is>
           <t>Fischer-Lichte, Erika (2008): The Transformative Power of Performance. A new aesthetics. London: Routledge, https://doi.org/10.4324/9780203894989</t>
         </is>
@@ -17365,14 +17557,14 @@
       </c>
     </row>
     <row r="141" ht="12" customHeight="1" s="17">
-      <c r="B141" s="21" t="inlineStr">
+      <c r="B141" s="22" t="inlineStr">
         <is>
           <t>Jogschies, Bärbel; Schewe, Manfred &amp; Stöver-Blahak, Anke (2018): Recommendations for the Promotion of a Performative Teaching and Learning Culture. In: Scenario XII/2, 52-56, http://publish.ucc.ie/journals/scenario/2018/02 [last accessed June 22, 2020]</t>
         </is>
       </c>
     </row>
     <row r="142" ht="12" customHeight="1" s="17">
-      <c r="B142" s="21" t="inlineStr">
+      <c r="B142" s="22" t="inlineStr">
         <is>
           <t>Piazzoli, Erika (2018): Embodying Language in Action. The Artistry of Process Drama in Second Language Education. Cham: Palgrave Macmillan,</t>
         </is>
@@ -17398,7 +17590,7 @@
       </c>
     </row>
     <row r="145" ht="12" customHeight="1" s="17">
-      <c r="B145" s="21" t="inlineStr">
+      <c r="B145" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Searle, John (1969): Speech Acts: An Essay in the Philosophy of Language. Cambridge: Cambridge University Press, </t>
         </is>
@@ -17410,14 +17602,14 @@
       </c>
     </row>
     <row r="146" ht="12" customHeight="1" s="17">
-      <c r="B146" s="21" t="inlineStr">
+      <c r="B146" s="22" t="inlineStr">
         <is>
           <t>UNESCO (2006): Road Map for Arts Education. The World Conference on Arts Education: Building Creative Capacities for the 21st Century. Lisbon, 6-9 March 2006, http://www.unesco.org/new/fileadmin/MULTIMEDIA/HQ/CLT/CLT/pdf/Arts_Edu_RoadMap_en.pdf [last accessed June 22, 2020]</t>
         </is>
       </c>
     </row>
     <row r="147" ht="12" customHeight="1" s="17">
-      <c r="B147" s="21" t="inlineStr">
+      <c r="B147" s="22" t="inlineStr">
         <is>
           <t>4th Scenario Forum Symposium Participants (2016): What exactly is an apple pie? Performative arts and pedagogy: Towards the development of an international glossary. In: Scenario X/2, 65-81, http://research.ucc.ie/scenario/2016/02 [last accessed June, 22 2020]</t>
         </is>
@@ -17469,7 +17661,7 @@
       </c>
     </row>
     <row r="153" ht="12" customHeight="1" s="17">
-      <c r="B153" s="21" t="inlineStr">
+      <c r="B153" s="22" t="inlineStr">
         <is>
           <t>Bundesministerium für Familie, Senioren, Frauen und Jugend (2016): Richtlinie über die Gewährung von Zuschüssen und Leistungen zur Förderung der Kinder- und Jugendhilfe durch den Kinder- und Jugendplan des Bundes (KJP). https://www.bmfsfj.de/blob/111964/2f7ae557daa0d2d8fe78f8a3f9569f21/richtlinien-kjp-2017-data.pdf [letzter Zugriff 3. April 2020]</t>
         </is>
@@ -17549,7 +17741,7 @@
       </c>
     </row>
     <row r="163" ht="12" customHeight="1" s="17">
-      <c r="B163" s="21" t="inlineStr">
+      <c r="B163" s="22" t="inlineStr">
         <is>
           <t>Heuer, Herbert (2020): Exekutive Funktionen. In: Wirtz, Markus (Hrsg.): Dorsch – Lexikon der Psychologie. https://portal.hogrefe.com/dorsch/exekutive-funktionen/ [letzter Zugriff 3. April 2020]</t>
         </is>
@@ -17584,7 +17776,7 @@
       </c>
     </row>
     <row r="168" ht="12" customHeight="1" s="17">
-      <c r="B168" s="21" t="inlineStr">
+      <c r="B168" s="22" t="inlineStr">
         <is>
           <t>Konferenz der Kultusminister der Länder / KMK (2013): Empfehlung der Kultusministerkonferenz zur kulturellen Kinder- und Jugendbildung. https://www.kmk.org/fileadmin/Dateien/pdf/Themen/Kultur/2007_02_01-Empfehlung-Kulturelle_Bildung.pdf [letzter Zugriff 3. April 2020]</t>
         </is>
@@ -17802,7 +17994,7 @@
       <c r="C225" s="1" t="n"/>
     </row>
     <row r="226" ht="12" customHeight="1" s="17">
-      <c r="B226" s="21" t="n"/>
+      <c r="B226" s="22" t="n"/>
     </row>
     <row r="227" ht="12" customHeight="1" s="17">
       <c r="B227" s="12" t="n"/>
@@ -17817,15 +18009,15 @@
       <c r="C229" s="1" t="n"/>
     </row>
     <row r="230" ht="12" customHeight="1" s="17">
-      <c r="B230" s="21" t="n"/>
+      <c r="B230" s="22" t="n"/>
       <c r="C230" s="1" t="n"/>
     </row>
     <row r="231" ht="12" customHeight="1" s="17">
-      <c r="B231" s="21" t="n"/>
+      <c r="B231" s="22" t="n"/>
       <c r="C231" s="1" t="n"/>
     </row>
     <row r="232" ht="12" customHeight="1" s="17">
-      <c r="B232" s="21" t="n"/>
+      <c r="B232" s="22" t="n"/>
     </row>
     <row r="233" ht="12" customHeight="1" s="17"/>
     <row r="234" ht="12" customHeight="1" s="17"/>
@@ -18698,10 +18890,10 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="24" customWidth="1" style="17" min="1" max="1"/>
-    <col width="8.86328125" customWidth="1" style="17" min="2" max="26"/>
+    <col width="8.85546875" customWidth="1" style="17" min="2" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="17">

</xml_diff>

<commit_message>
handle scenario snags, e.g. guest editors, page numbers etc
</commit_message>
<xml_diff>
--- a/contribs.xlsx
+++ b/contribs.xlsx
@@ -10623,7 +10623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G253"/>
+  <dimension ref="A1:G255"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
@@ -15457,8 +15457,44 @@
         </is>
       </c>
     </row>
-    <row r="254" ht="12.75" customHeight="1" s="17"/>
-    <row r="255" ht="12.75" customHeight="1" s="17"/>
+    <row r="254" ht="12.75" customHeight="1" s="17">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>theeditors</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>The</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Editors</t>
+        </is>
+      </c>
+    </row>
+    <row r="255" ht="12.75" customHeight="1" s="17">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>mandycollins</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Mandy</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Collins</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr"/>
+      <c r="E255" t="inlineStr"/>
+      <c r="F255" t="inlineStr"/>
+      <c r="G255" t="inlineStr"/>
+    </row>
     <row r="256" ht="12.75" customHeight="1" s="17"/>
     <row r="257" ht="12.75" customHeight="1" s="17"/>
     <row r="258" ht="12.75" customHeight="1" s="17"/>

</xml_diff>

<commit_message>
improve pdf modification. Add url_path attribute for galleys
</commit_message>
<xml_diff>
--- a/contribs.xlsx
+++ b/contribs.xlsx
@@ -15490,10 +15490,6 @@
           <t>Collins</t>
         </is>
       </c>
-      <c r="D255" t="inlineStr"/>
-      <c r="E255" t="inlineStr"/>
-      <c r="F255" t="inlineStr"/>
-      <c r="G255" t="inlineStr"/>
     </row>
     <row r="256" ht="12.75" customHeight="1" s="17"/>
     <row r="257" ht="12.75" customHeight="1" s="17"/>

</xml_diff>